<commit_message>
Fix: Chapter 1 Finish Test
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2026\C++\Signal_Lost\Signal_Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E204C4-4303-4CB4-81F5-528D10E040F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6258BEFC-2CEB-49D2-8E97-B2383C83F9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters_Header" sheetId="3" r:id="rId1"/>
@@ -109,12 +109,6 @@
 Now, I'm going to cross to the other side to see if there's anything in that part of town.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I found this phone in the supermarket, and simply opening it started a call.[Wait=500][Space=2]
-*Button presses*[Wait=500][Space=2]
-It doesn't seem to have any apps installed, I can't even access the contacts.[Wait=500][Space=2]
-Calling you was the only thing I could do with this dusty relic of a device.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>There's no certainty... This place feels so empty. Hauntingly empty, the unnatural kind of loneliness...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 I'm being dramatic for a reason.[Wait=500] It's chilling.[Wait=500] Something's wrong with this place.[Wait=500][Space=2]</t>
@@ -462,15 +456,6 @@
 [Color=Gray]*You hear a quiet breath and the mechanical noise slowly becoming louder*[Color=White]...[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I see... A door down the hall.[Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
-I hear some sound behind it...[Wait=500] What do I do?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>ALRIGHT, I'LL TYPE THIS...[Wait=500][Space=2]
-Oh...[Wait=500] Looks like the beeping sound sto-[Wait=500] [Color=Gray]*BOOOM*[Color=White][Wait=500] [Color=Gray]*SHKRRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I'm going to go and see if that's really what happened...[Wait=500][Space=2]
 Damn,[Wait=500] I wonder what would have happened if we didn't type the password in time.[Wait=500][Space=2]
 It might be better to forget about it right now.[Wait=500][Space=2]
@@ -660,13 +645,6 @@
 I'm sorry to take your time like that, but I haven't really got a choice.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>O-Okay! I gotta get out of the building first, just stay with me.[Wait=500][Space=2]
-[Color=Gray]*You hear the person’s footsteps echoing through the supermarket*[Color=White]...[Wait=500][Space=2]
-This place is huge, you don’t realize that until the mall’s empty.[Wait=500] Just, what happened he-[Wait=500][Space=2]
-...[Wait=500][Space=2]
-I hear something.[Wait=500] Mechanical, screeching kind of noise.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I've been exploring this island for hours now and I've found nothing back where I was.[Wait=500][Space=2]
 It's the first time I hear anything other than the wind or the waves hitting the shore.[Wait=500][Space=2]
 So I'm not turning my back now.[Wait=500][Space=2]
@@ -685,14 +663,6 @@
 Damn me, I'm making up the worst scenarios in my head now.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Hum...[Wait=500][Space=2]
-Okay? It might lead somewhere interesting.[Wait=500][Space=2]
-I just have to...[Wait=500] Take a step at the right...[Wait=500] Time...[Wait=500][Space=2]
-WOOAAH SHI-[Color=Gray]*THUMP*[Color=White]...[Wait=500][Space=2]
-...[Wait=500][Space=2]
-...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>...[Wait=500][Space=2]
 Ouch...[Wait=500][Space=2]
 That hurt as hell...[Wait=500][Space=2]
@@ -719,13 +689,6 @@
 Let's not be stupid and find a way up here without getting hurt.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Okay![Wait=500] I'm hungry as hell, I wouldn't say no to a little snack.[Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*Sniff*[Color=White][Wait=500] OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
-Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
-[Color=Gray]*Glurp*[Color=White][Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Right, let's go![Wait=500] A good hammer is always useful, especially in the kind of situation I'm in, I guess.[Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
 ...Alright! Here I am.[Wait=500][Space=2]
@@ -739,36 +702,10 @@
 There is some door-wedge and packs of rusty nails...[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>You sure?[Wait=500] I mean, I'm hungry as hell, so I might take a bite if there was anything to eat.[Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Sniff*[Color=White]...[Wait=500][Space=2]
-OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
-Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
-[Color=Gray]*Glurp*[Color=White][Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Y-You're right... It's best to get out of here before I-...[Wait=500] [Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
 ...Oof, one more second and I think I would have passed out.[Wait=500] Anyway, here I am.[Wait=500][Space=2]
 There are far fewer things on the shelves than I imagined.[Wait=500][Space=2]
 There is some door-wedge and rusty nails...[Wait=500] Nothing that could be useful in the end.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Yeah, I guess, but it's on-[Color=Gray]*Glurp*[Color=White]...[Wait=500] Only because you asked me nicely...[Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White]...[Wait=500] Good heavens, aren't these trash supposed to be eaten by the bugs?[Wait=500][Space=2]
-Wait?[Wait=500] There's a cereal bar over here that still is good to eat![Wait=500][Space=2]
-[Color=Gray]*Crunch*[Color=White][Wait=500] Yum... That’s good to eat something...[Wait=500] [Color=Gray]*Gulp*[Color=White][Wait=500] Ah yes, I needed that.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Alright. Let's do it the hard way.[Wait=500][Space=2]
-[Color=Gray]*KICK*[Color=White][Wait=500] POLICE, DON'T MOVE![Wait=500] Ouch ouch ouch! My foot hurt as hell now...[Wait=500][Space=2]
-Great! The door was clearly open! And there's no one here anyway... This door wasn't worth kicking.[Wait=500][Space=2]
-It's just a security room.[Wait=500] Everything seems out of pow-.[Wait=500][Space=2]
-...Oh my bad, seems to be one thing still working![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Okay... Carefully...[Wait=500][Space=2]
-...[Wait=500] Well, there is clearly no one here.[Wait=500][Space=2]
-It's an old security room, everything is out of power.[Wait=500][Space=2]
-Oh no, my bad, the beeping sound is coming from here![Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Let me see...[Wait=500] Ah AH![Wait=500] There's a door over here![Wait=500][Space=2]
@@ -804,21 +741,8 @@
 There's a huge "EXIT" word tagged on it.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>AHAHAHAH![Wait=500] You're right![Wait=500][Space=2]
-Now, how do I open this thing?[Wait=500][Space=2]
-There are no visible handles, and it looks far too resistant to be opened with my bare hands.[Wait=500][Space=2]
-Please tell me tha-... Oh![Wait=500] There's a command panel over here![Wait=500][Space=2]
-...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Y-You might be right, but that's the first time I see something that brings me hope of getting out of here.[Wait=500][Space=2]
 If there is even a single chance that this trapdoor brings me back to civilization, I'll do everything to open it.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Well… There's no handle attached to it anywhere...[Wait=500][Space=2]
-HNNG![Wait=500] Huff...[Wait=500] I can't open it with my bare hands either.[Wait=500][Space=2]
-It seems locked by some kind of electrical mechanism that leads to this control panel.[Wait=500][Space=2]
-...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>No, I checked pretty much every shelf while I was inside, and there was nothing but dust on them.[Wait=500][Space=2]
@@ -851,13 +775,6 @@
     <t>Hmmm... The buildings here look exactly the same compared to the ones I crossed before calling you...[Wait=500][Space=2]
 Hey![Wait=500] There are signs leading to two different locations here.[Wait=500][Space=2]
 One is leading to a [Color=Green]"Factory"[Color=White] and the other to a [Color=Green]"Zoo"[Color=White].[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I-It's uuuuh...[Wait=500] A laptop, seems to be on the lockscreen.[Wait=500][Space=2]
-There's a post-it attached on the upper right corner of it.[Wait=500] It says [Color=Green]"Vaccine Rabies Year"[Color=White]...[Wait=500][Space=2]
-I don't know when that thing was![Wait=500][Space=2]
-...What?[Wait=500] I don't remember how I got here in the first place, don't expect me to remember this![Wait=500][Space=2]
-Anyway, you might want to search for that on the internet, it's a 4-digit password.[Wait=500] I'll try to log in.[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>[Choice1=[NextScene=13][Content=Why are you doubting all of a sudden?]]
@@ -1103,12 +1020,6 @@
     <t>[Choice1=[NextScene=107][Content=See you later.]]</t>
   </si>
   <si>
-    <t>[Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*SHKRRRRRRRRR*[Color=White]...H-Hello? Is someone there-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
-How does this thing wor-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] Can you hear m-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
-Hello?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Color=Gray]*SHKRRRRRR*[Color=White]-MY GOD! I’ve been stuck here-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-for days. It feels so good to hear someone’s voice...[Wait=500][Space=2]
 [Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-Any idea what’s happening? Who are y-[Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-I, and why am I here?[Wait=500][Space=2]</t>
   </si>
@@ -1116,13 +1027,6 @@
     <t>Can’t even tell! I just found this old flip phone on a shelf.[Wait=500][Space=2]
 It started a call the moment I opened it![Wait=500][Space=2]
 There's nothing else on that piece of junk, no contacts, no internet access, just this call number.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>PLEASE DON’T HANG UP! I just need someone to talk to![Wait=500][Space=2]
-I have no idea if either of us will even be able to call again if you hang up![Wait=500][Space=2]
-Wh-[Wait=500] whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
-...[Wait=500][Space=2]
-[Color=Magenta][Beep=True]It[Wait=500][Beep=True] wO[Wait=500][Beep=True] uLd[Wait=500][Beep=True] bE uS[Wait=500][Beep=True] eLLeSs.[Wait=500][Beep=True] Ke[Wait=500][Beep=True] p tHe[Wait=500][Beep=True] CaLL[Wait=500][Beep=True] gO[Wait=500][Beep=True] iNg.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Going to the museum?[Wait=500] I can work with that.[Wait=500][Space=2]
@@ -2466,6 +2370,102 @@
 [Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
 [Color=Red]{HE CAUGHT HIM. WAS THERE NO OTHER CHOICE?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*SHKRRRRRRRRR*[Color=White]...[Wait=500] H-Hello? Is someone there-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+How does this thing wor-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] Can you hear m-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+Hello?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I found this phone in the supermarket, and simply opening it started a call.[Wait=500][Space=2]
+[Color=Gray]*Button press*[Color=White]...[Wait=500][Space=2]
+It doesn't seem to have any apps installed, I can't even access the contacts.[Wait=500][Space=2]
+Calling you was the only thing I could do with this dusty relic of a device.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>PLEASE DON’T HANG UP! I just need someone to talk to![Wait=500][Space=2]
+I have no idea if either of us will even be able to call again if you hang up![Wait=500][Space=2]
+Wh-[Wait=500] Whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
+...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]It[Wait=500][Beep=True] wO[Wait=500][Beep=True] uLd[Wait=500][Beep=True] bE uS[Wait=500][Beep=True] eLLeSs.[Wait=500][Beep=True] Ke[Wait=500][Beep=True] p tHe[Wait=500][Beep=True] CaLL[Wait=500][Beep=True] gO[Wait=500][Beep=True] iNg.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>O-Okay! I gotta get out of the building first, just stay with me.[Wait=500][Space=2]
+[Color=Gray]*You hear the person’s footsteps echoing through the supermarket*[Color=White]...[Wait=500][Space=2]
+This place is huge, you don’t realize that until the mall’s empty.[Wait=500] Just, what happened he-...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I hear something.[Wait=500] Mechanical, screeching kind of noise.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Hum...[Wait=500][Space=2]
+Okay? It might lead somewhere interesting.[Wait=500][Space=2]
+I just have to...[Wait=500] take a step at the right...[Wait=500] time...[Wait=500][Space=2]
+WOOAAH SHI-[Color=Gray]*THUMP*[Color=White]...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Okay![Wait=500] I'm hungry as hell, I wouldn't say no to a little snack.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*Sniff*[Color=White]...[Wait=500] OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
+Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
+[Color=Gray]*Glurp*[Color=White]...[Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You sure?[Wait=500] I mean, I'm hungry as hell, so I might take a bite if there was anything to eat.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Sniff*[Color=White]...[Wait=500][Space=2]
+OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
+Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
+[Color=Gray]*Glurp*[Color=White]...[Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah, I guess, but it's on-[Color=Gray]*Glurp*[Color=White]...[Wait=500] Only because you asked me nicely...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] Good heavens, aren't these trash supposed to be eaten by the bugs?[Wait=500][Space=2]
+Wait?[Wait=500] There's a cereal bar over here that still is good to eat![Wait=500][Space=2]
+[Color=Gray]*Crunch*[Color=White]...[Wait=500] Yum... That’s good to eat something...[Wait=500] [Color=Gray]*Gulp*[Color=White]...[Wait=500] Ah yes, I needed that.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I see... a door down the hall.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+I hear some sound behind it...[Wait=500] What do I do?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Alright. Let's do it the hard way.[Wait=500][Space=2]
+[Color=Gray]*KICK*[Color=White]...[Wait=500] POLICE, DON'T MOVE![Wait=500] Ouch ouch ouch! My foot hurt as hell now...[Wait=500][Space=2]
+Great! The door was clearly open! And there's no one here anyway... This door wasn't worth kicking.[Wait=500][Space=2]
+It's just a security room.[Wait=500] Everything seems out of pow-.[Wait=500][Space=2]
+...Oh my bad, seems to be one thing still working![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Okay... carefully...[Wait=500][Space=2]
+...[Wait=500] Well, there is clearly no one here.[Wait=500][Space=2]
+It's an old security room, everything is out of power.[Wait=500][Space=2]
+Oh no, my bad, the beeping sound is coming from here![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I-It's uuuuh...[Wait=500] A laptop, seems to be on the lockscreen.[Wait=500][Space=2]
+There's a post-it attached on the upper right corner of it.[Wait=500] It says [Color=Green]"Vaccine Rabies Year"[Color=White]...[Wait=500][Space=2]
+I don't know when that thing was![Wait=500][Space=2]
+...What?[Wait=500] I don't remember how I got here in the first place, don't expect me to remember this![Wait=500][Space=2]
+Anyway, you might want to search for that on the internet, it's a [Color=Green]4-digit password[Color=White].[Wait=500] I'll try to log in.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>ALRIGHT, I'LL TYPE THIS...[Wait=500][Space=2]
+Oh...[Wait=500] Looks like the beeping sound sto-[Color=Gray]*BOOOM*[Color=White]...[Wait=500] [Color=Gray]*SHKRRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>AHAHAHAH![Wait=500] You're right![Wait=500][Space=2]
+Now, how do I open this thing?[Wait=500][Space=2]
+There are no visible handles, and it looks far too resistant to be opened with my bare hands.[Wait=500][Space=2]
+Please tell me tha-...[Wait=500] Oh![Wait=500] There's a command panel over here![Wait=500][Space=2]
+...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Well...[Wait=500] There's no handle attached to it anywhere...[Wait=500][Space=2]
+HNNG![Wait=500] Huff...[Wait=500] I can't open it with my bare hands either.[Wait=500][Space=2]
+It seems locked by some kind of electrical mechanism that leads to this control panel.[Wait=500][Space=2]
+...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
   </si>
 </sst>
 </file>
@@ -4983,7 +4983,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C2" s="12">
         <v>4</v>
@@ -5000,7 +5000,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="12">
         <v>3</v>
@@ -5017,7 +5017,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="12">
         <v>3</v>
@@ -5034,7 +5034,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="12">
         <v>3</v>
@@ -5099,8 +5099,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="B66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5121,7 +5121,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -5133,7 +5133,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5150,10 +5150,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="23" t="str">
         <f>"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -5180,7 +5180,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>240</v>
+        <v>471</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
@@ -5191,7 +5191,7 @@
 [Connection=1]
 [Content=
 [Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*SHKRRRRRRRRR*[Color=White]...H-Hello? Is someone there-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*SHKRRRRRRRRR*[Color=White]...[Wait=500] H-Hello? Is someone there-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 How does this thing wor-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] Can you hear m-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 Hello?[Wait=500][Space=2]
 ]
@@ -5211,10 +5211,10 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5243,10 +5243,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5270,10 +5270,10 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5299,10 +5299,10 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5330,10 +5330,10 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5362,7 +5362,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5387,10 +5387,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5417,10 +5417,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5446,10 +5446,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5475,10 +5475,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5506,7 +5506,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5530,10 +5530,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5560,10 +5560,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5587,17 +5587,17 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>18</v>
+        <v>472</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=16
 [Content=
 I found this phone in the supermarket, and simply opening it started a call.[Wait=500][Space=2]
-*Button presses*[Wait=500][Space=2]
+[Color=Gray]*Button press*[Color=White]...[Wait=500][Space=2]
 It doesn't seem to have any apps installed, I can't even access the contacts.[Wait=500][Space=2]
 Calling you was the only thing I could do with this dusty relic of a device.[Wait=500][Space=2]
 ]
@@ -5616,10 +5616,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5644,10 +5644,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5672,10 +5672,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5702,10 +5702,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5731,10 +5731,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5763,10 +5763,10 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>243</v>
+        <v>473</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5775,7 +5775,7 @@
 [Content=
 PLEASE DON’T HANG UP! I just need someone to talk to![Wait=500][Space=2]
 I have no idea if either of us will even be able to call again if you hang up![Wait=500][Space=2]
-Wh-[Wait=500] whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
+Wh-[Wait=500] Whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
 ...[Wait=500][Space=2]
 [Color=Magenta][Beep=True]It[Wait=500][Beep=True] wO[Wait=500][Beep=True] uLd[Wait=500][Beep=True] bE uS[Wait=500][Beep=True] eLLeSs.[Wait=500][Beep=True] Ke[Wait=500][Beep=True] p tHe[Wait=500][Beep=True] CaLL[Wait=500][Beep=True] gO[Wait=500][Beep=True] iNg.[Color=White][Wait=500][Space=2]
 ]
@@ -5796,10 +5796,10 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5833,7 +5833,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5861,10 +5861,10 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5893,10 +5893,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5920,10 +5920,10 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5947,10 +5947,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>143</v>
+        <v>474</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5958,7 +5958,7 @@
 [Content=
 O-Okay! I gotta get out of the building first, just stay with me.[Wait=500][Space=2]
 [Color=Gray]*You hear the person’s footsteps echoing through the supermarket*[Color=White]...[Wait=500][Space=2]
-This place is huge, you don’t realize that until the mall’s empty.[Wait=500] Just, what happened he-[Wait=500][Space=2]
+This place is huge, you don’t realize that until the mall’s empty.[Wait=500] Just, what happened he-...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 I hear something.[Wait=500] Mechanical, screeching kind of noise.[Wait=500][Space=2]
 ]
@@ -5977,10 +5977,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6006,10 +6006,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6034,10 +6034,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6063,10 +6063,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6093,10 +6093,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -6123,10 +6123,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6155,10 +6155,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6187,10 +6187,10 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>147</v>
+        <v>475</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6199,7 +6199,7 @@
 [Content=
 Hum...[Wait=500][Space=2]
 Okay? It might lead somewhere interesting.[Wait=500][Space=2]
-I just have to...[Wait=500] Take a step at the right...[Wait=500] Time...[Wait=500][Space=2]
+I just have to...[Wait=500] take a step at the right...[Wait=500] time...[Wait=500][Space=2]
 WOOAAH SHI-[Color=Gray]*THUMP*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
@@ -6220,10 +6220,10 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6251,10 +6251,10 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6279,10 +6279,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6308,10 +6308,10 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6337,10 +6337,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>152</v>
+        <v>476</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6348,9 +6348,9 @@
 [Content=
 Okay![Wait=500] I'm hungry as hell, I wouldn't say no to a little snack.[Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*Sniff*[Color=White][Wait=500] OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
+[Color=Gray]*Sniff*[Color=White]...[Wait=500] OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
 Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
-[Color=Gray]*Glurp*[Color=White][Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]
+[Color=Gray]*Glurp*[Color=White]...[Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=45][Content=Maybe it’s a better idea to check out the craft section...]]
@@ -6367,10 +6367,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6396,10 +6396,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6424,10 +6424,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>155</v>
+        <v>477</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6437,7 +6437,7 @@
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Sniff*[Color=White]...[Wait=500][Space=2]
 OH G-...[Wait=500] IT SMELLS TERRIBLE OVER HERE![Wait=500][Space=2]
 Shelves are filled with rotten fruits and vegeta-...[Wait=500][Space=2]
-[Color=Gray]*Glurp*[Color=White][Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]
+[Color=Gray]*Glurp*[Color=White]...[Wait=500] Oh lord, I almost threw up...[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=46][Content=Can you keep going? There might be something interesting here.]]
@@ -6453,10 +6453,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6481,10 +6481,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>157</v>
+        <v>478</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6493,7 +6493,7 @@
 Yeah, I guess, but it's on-[Color=Gray]*Glurp*[Color=White]...[Wait=500] Only because you asked me nicely...[Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] Good heavens, aren't these trash supposed to be eaten by the bugs?[Wait=500][Space=2]
 Wait?[Wait=500] There's a cereal bar over here that still is good to eat![Wait=500][Space=2]
-[Color=Gray]*Crunch*[Color=White][Wait=500] Yum... That’s good to eat something...[Wait=500] [Color=Gray]*Gulp*[Color=White][Wait=500] Ah yes, I needed that.[Wait=500][Space=2]
+[Color=Gray]*Crunch*[Color=White]...[Wait=500] Yum... That’s good to eat something...[Wait=500] [Color=Gray]*Gulp*[Color=White]...[Wait=500] Ah yes, I needed that.[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=50][Content=Are you finished eating? Is there anything else here?]]
@@ -6509,16 +6509,16 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>104</v>
+        <v>479</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=47
 [Content=
-I see... A door down the hall.[Wait=500][Space=2]
+I see... a door down the hall.[Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
 I hear some sound behind it...[Wait=500] What do I do?[Wait=500][Space=2]
 ]
@@ -6537,17 +6537,17 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>158</v>
+        <v>480</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=48
 [Content=
 Alright. Let's do it the hard way.[Wait=500][Space=2]
-[Color=Gray]*KICK*[Color=White][Wait=500] POLICE, DON'T MOVE![Wait=500] Ouch ouch ouch! My foot hurt as hell now...[Wait=500][Space=2]
+[Color=Gray]*KICK*[Color=White]...[Wait=500] POLICE, DON'T MOVE![Wait=500] Ouch ouch ouch! My foot hurt as hell now...[Wait=500][Space=2]
 Great! The door was clearly open! And there's no one here anyway... This door wasn't worth kicking.[Wait=500][Space=2]
 It's just a security room.[Wait=500] Everything seems out of pow-.[Wait=500][Space=2]
 ...Oh my bad, seems to be one thing still working![Wait=500][Space=2]
@@ -6566,16 +6566,16 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>159</v>
+        <v>481</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=49
 [Content=
-Okay... Carefully...[Wait=500][Space=2]
+Okay... carefully...[Wait=500][Space=2]
 ...[Wait=500] Well, there is clearly no one here.[Wait=500][Space=2]
 It's an old security room, everything is out of power.[Wait=500][Space=2]
 Oh no, my bad, the beeping sound is coming from here![Wait=500][Space=2]
@@ -6594,10 +6594,10 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6623,10 +6623,10 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>175</v>
+        <v>482</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6636,7 +6636,7 @@
 There's a post-it attached on the upper right corner of it.[Wait=500] It says [Color=Green]"Vaccine Rabies Year"[Color=White]...[Wait=500][Space=2]
 I don't know when that thing was![Wait=500][Space=2]
 ...What?[Wait=500] I don't remember how I got here in the first place, don't expect me to remember this![Wait=500][Space=2]
-Anyway, you might want to search for that on the internet, it's a 4-digit password.[Wait=500] I'll try to log in.[Wait=500][Space=2]
+Anyway, you might want to search for that on the internet, it's a [Color=Green]4-digit password[Color=White].[Wait=500] I'll try to log in.[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=52][Content=Okay, go ahead, I'm going to search that in my browser.]]
@@ -6656,10 +6656,10 @@
         <v>60</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6693,10 +6693,10 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>105</v>
+        <v>483</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6704,7 +6704,7 @@
 [Connection=1]
 [Content=
 ALRIGHT, I'LL TYPE THIS...[Wait=500][Space=2]
-Oh...[Wait=500] Looks like the beeping sound sto-[Wait=500] [Color=Gray]*BOOOM*[Color=White][Wait=500] [Color=Gray]*SHKRRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+Oh...[Wait=500] Looks like the beeping sound sto-[Color=Gray]*BOOOM*[Color=White]...[Wait=500] [Color=Gray]*SHKRRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=54][Content=Are you here?]]
@@ -6722,10 +6722,10 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6759,7 +6759,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6787,10 +6787,10 @@
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6815,10 +6815,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6843,10 +6843,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6872,10 +6872,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6900,10 +6900,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6927,10 +6927,10 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6955,10 +6955,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6983,10 +6983,10 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>166</v>
+        <v>484</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6995,7 +6995,7 @@
 AHAHAHAH![Wait=500] You're right![Wait=500][Space=2]
 Now, how do I open this thing?[Wait=500][Space=2]
 There are no visible handles, and it looks far too resistant to be opened with my bare hands.[Wait=500][Space=2]
-Please tell me tha-... Oh![Wait=500] There's a command panel over here![Wait=500][Space=2]
+Please tell me tha-...[Wait=500] Oh![Wait=500] There's a command panel over here![Wait=500][Space=2]
 ...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]
 ]
 [Choices=
@@ -7012,10 +7012,10 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
@@ -7038,16 +7038,16 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>168</v>
+        <v>485</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G74" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=65
 [Content=
-Well… There's no handle attached to it anywhere...[Wait=500][Space=2]
+Well...[Wait=500] There's no handle attached to it anywhere...[Wait=500][Space=2]
 HNNG![Wait=500] Huff...[Wait=500] I can't open it with my bare hands either.[Wait=500][Space=2]
 It seems locked by some kind of electrical mechanism that leads to this control panel.[Wait=500][Space=2]
 ...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]
@@ -7069,7 +7069,7 @@
         <v>14</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7095,10 +7095,10 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7126,10 +7126,10 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7155,10 +7155,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7184,10 +7184,10 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7211,10 +7211,10 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7243,10 +7243,10 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7275,7 +7275,7 @@
         <v>15</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G74" s="24" t="str">
         <f t="shared" si="2"/>
@@ -7351,7 +7351,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -7363,7 +7363,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7376,10 +7376,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -7403,10 +7403,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7432,10 +7432,10 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7459,10 +7459,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7488,10 +7488,10 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7516,10 +7516,10 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7543,10 +7543,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7570,10 +7570,10 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7598,10 +7598,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7627,10 +7627,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7655,10 +7655,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7682,10 +7682,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7709,10 +7709,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7737,10 +7737,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7764,10 +7764,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7793,10 +7793,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7822,10 +7822,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7851,10 +7851,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7880,10 +7880,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7909,10 +7909,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7936,10 +7936,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7964,10 +7964,10 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7990,10 +7990,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8017,10 +8017,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8044,10 +8044,10 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8072,10 +8072,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8100,10 +8100,10 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8129,10 +8129,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8156,10 +8156,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8183,10 +8183,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8210,10 +8210,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8237,10 +8237,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8266,10 +8266,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -8294,10 +8294,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8326,10 +8326,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8357,10 +8357,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8383,10 +8383,10 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8409,10 +8409,10 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8435,10 +8435,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8462,10 +8462,10 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8490,10 +8490,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8518,10 +8518,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8545,10 +8545,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8573,10 +8573,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8601,10 +8601,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8628,10 +8628,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8658,10 +8658,10 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8690,10 +8690,10 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8724,10 +8724,10 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8756,10 +8756,10 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8788,10 +8788,10 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8820,10 +8820,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8849,10 +8849,10 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8878,10 +8878,10 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8907,10 +8907,10 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8934,10 +8934,10 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8960,10 +8960,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8986,10 +8986,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9014,10 +9014,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9041,10 +9041,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9069,10 +9069,10 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9096,10 +9096,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9123,10 +9123,10 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9151,10 +9151,10 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9180,10 +9180,10 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G97" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -9208,10 +9208,10 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9235,10 +9235,10 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9262,10 +9262,10 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9289,10 +9289,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9318,10 +9318,10 @@
         <v>7</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9348,10 +9348,10 @@
         <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9378,10 +9378,10 @@
         <v>7</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9406,10 +9406,10 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="8" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G74" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9436,10 +9436,10 @@
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="G75" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9464,10 +9464,10 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G76" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9490,10 +9490,10 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G77" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9516,10 +9516,10 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G78" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9542,10 +9542,10 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G79" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9570,10 +9570,10 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="G80" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9599,10 +9599,10 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="G81" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9627,10 +9627,10 @@
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="G82" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9655,10 +9655,10 @@
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="8" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="G83" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9682,10 +9682,10 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="G84" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9709,10 +9709,10 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="G85" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9736,10 +9736,10 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="G86" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9765,10 +9765,10 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="G87" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9793,10 +9793,10 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9821,10 +9821,10 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G89" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9849,10 +9849,10 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G90" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9880,10 +9880,10 @@
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="G91" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9912,10 +9912,10 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="G92" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9945,10 +9945,10 @@
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G93" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9981,10 +9981,10 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="G94" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10011,10 +10011,10 @@
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="G95" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10037,10 +10037,10 @@
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="G96" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10067,10 +10067,10 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="G97" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10096,10 +10096,10 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="G98" s="23" t="str">
         <f t="shared" ref="G98:G108" si="3">"[Scene=" &amp; A98 &amp; IF(OR(B98&lt;&gt;"",C98&lt;&gt;"",D98&lt;&gt;""),CHAR(10),"") &amp; IF(B98&lt;&gt;"","[BeepBack=" &amp; B98 &amp; "]","") &amp; IF(C98&lt;&gt;"","[Connection=" &amp; C98 &amp; "]","") &amp; IF(D98&lt;&gt;"","[Timer=" &amp; D98 &amp; "]","") &amp; IF(E98&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E98 &amp; CHAR(10) &amp; "]","") &amp; IF(F98&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F98 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -10127,10 +10127,10 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="G99" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10158,10 +10158,10 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10192,10 +10192,10 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="G101" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10223,10 +10223,10 @@
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="G102" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10255,10 +10255,10 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="G103" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10287,10 +10287,10 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="G104" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10316,10 +10316,10 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="G105" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10344,10 +10344,10 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10373,10 +10373,10 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G107" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10403,10 +10403,10 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G108" s="24" t="str">
         <f t="shared" si="3"/>
@@ -10468,7 +10468,7 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
@@ -10490,7 +10490,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -10502,7 +10502,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10515,7 +10515,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="23" t="str">
@@ -10538,7 +10538,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="23" t="str">
@@ -10561,7 +10561,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="23" t="str">
@@ -10582,7 +10582,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="23" t="str">
@@ -10606,7 +10606,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="23" t="str">
@@ -10629,7 +10629,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="23" t="str">
@@ -10653,7 +10653,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="23" t="str">
@@ -10678,7 +10678,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="23" t="str">
@@ -10702,7 +10702,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="23" t="str">
@@ -10727,7 +10727,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="23" t="str">
@@ -10749,7 +10749,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="23" t="str">
@@ -10772,7 +10772,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="23" t="str">
@@ -10794,7 +10794,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="23" t="str">
@@ -10816,7 +10816,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="23" t="str">
@@ -10837,7 +10837,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="23" t="str">
@@ -10862,7 +10862,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="23" t="str">
@@ -10887,7 +10887,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="23" t="str">
@@ -10911,7 +10911,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="23" t="str">
@@ -10932,7 +10932,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="23" t="str">
@@ -10955,7 +10955,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="23" t="str">
@@ -10976,7 +10976,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="23" t="str">
@@ -10998,7 +10998,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="23" t="str">
@@ -11021,7 +11021,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="23" t="str">
@@ -11045,7 +11045,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="23" t="str">
@@ -11069,7 +11069,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="23" t="str">
@@ -11094,7 +11094,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="23" t="str">
@@ -11117,7 +11117,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="23" t="str">
@@ -11140,7 +11140,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="23" t="str">
@@ -11163,7 +11163,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="23" t="str">
@@ -11187,7 +11187,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="23" t="str">
@@ -11210,7 +11210,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="23" t="str">
@@ -11233,7 +11233,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="23" t="str">
@@ -11255,7 +11255,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="23" t="str">
@@ -11278,7 +11278,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="23" t="str">
@@ -11300,7 +11300,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="23" t="str">
@@ -11324,7 +11324,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="23" t="str">
@@ -11347,7 +11347,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="23" t="str">
@@ -11373,7 +11373,7 @@
         <v>60</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="23" t="str">
@@ -11399,7 +11399,7 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="23" t="str">
@@ -11427,7 +11427,7 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="23" t="str">
@@ -11456,7 +11456,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="23" t="str">
@@ -11482,7 +11482,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="23" t="str">
@@ -11504,7 +11504,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="23" t="str">
@@ -11527,7 +11527,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="23" t="str">
@@ -11550,7 +11550,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="23" t="str">
@@ -11572,7 +11572,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="23" t="str">
@@ -11596,7 +11596,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="23" t="str">
@@ -11618,7 +11618,7 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="23" t="str">
@@ -11646,7 +11646,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="23" t="str">
@@ -11669,7 +11669,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="23" t="str">
@@ -11690,7 +11690,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="23" t="str">
@@ -11713,7 +11713,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="23" t="str">
@@ -11737,7 +11737,7 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="23" t="str">
@@ -11759,7 +11759,7 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="23" t="str">
@@ -11781,7 +11781,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="23" t="str">
@@ -11803,7 +11803,7 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="23" t="str">
@@ -11825,7 +11825,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="23" t="str">
@@ -11847,7 +11847,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="23" t="str">
@@ -11873,7 +11873,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="23" t="str">
@@ -11895,7 +11895,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="23" t="str">
@@ -11916,7 +11916,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="23" t="str">
@@ -11939,7 +11939,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="23" t="str">
@@ -11961,7 +11961,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="23" t="str">
@@ -11982,7 +11982,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="23" t="str">
@@ -12007,7 +12007,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="23" t="str">
@@ -12034,7 +12034,7 @@
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="23" t="str">
@@ -12061,7 +12061,7 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="23" t="str">
@@ -12087,7 +12087,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="23" t="str">
@@ -12110,7 +12110,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="23" t="str">
@@ -12132,7 +12132,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="23" t="str">
@@ -12156,7 +12156,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="23" t="str">
@@ -12179,7 +12179,7 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="F73" s="8"/>
       <c r="G73" s="23" t="str">
@@ -12202,7 +12202,7 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="F74" s="13"/>
       <c r="G74" s="24" t="str">
@@ -12225,7 +12225,7 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="23" t="str">
@@ -12246,7 +12246,7 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="23" t="str">
@@ -12268,7 +12268,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="23" t="str">
@@ -12291,7 +12291,7 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="23" t="str">
@@ -12313,7 +12313,7 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="23" t="str">
@@ -12336,7 +12336,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="23" t="str">
@@ -12359,7 +12359,7 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="23" t="str">
@@ -12384,7 +12384,7 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="23" t="str">
@@ -12410,7 +12410,7 @@
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="24" t="str">
@@ -12437,7 +12437,7 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="F84" s="8"/>
       <c r="G84" s="23" t="str">
@@ -12461,7 +12461,7 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="F85" s="8"/>
       <c r="G85" s="23" t="str">
@@ -12483,7 +12483,7 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="F86" s="8"/>
       <c r="G86" s="23" t="str">
@@ -12505,7 +12505,7 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="F87" s="8"/>
       <c r="G87" s="23" t="str">
@@ -12527,7 +12527,7 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="23" t="str">
@@ -12550,7 +12550,7 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="F89" s="8"/>
       <c r="G89" s="23" t="str">
@@ -12572,7 +12572,7 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="23" t="str">
@@ -12595,7 +12595,7 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="23" t="str">
@@ -12619,7 +12619,7 @@
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="24" t="str">
@@ -12647,7 +12647,7 @@
         <v>10</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="F93" s="8"/>
       <c r="G93" s="23" t="str">
@@ -12673,7 +12673,7 @@
         <v>10</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="23" t="str">
@@ -12698,7 +12698,7 @@
         <v>10</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="F95" s="8"/>
       <c r="G95" s="23" t="str">
@@ -12725,7 +12725,7 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="F96" s="8"/>
       <c r="G96" s="23" t="str">
@@ -12750,7 +12750,7 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="F97" s="8"/>
       <c r="G97" s="23" t="str">
@@ -12775,7 +12775,7 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="F98" s="8"/>
       <c r="G98" s="23" t="str">
@@ -12800,7 +12800,7 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="F99" s="8"/>
       <c r="G99" s="23" t="str">
@@ -12826,7 +12826,7 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="F100" s="8"/>
       <c r="G100" s="23" t="str">
@@ -12852,7 +12852,7 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="F101" s="8"/>
       <c r="G101" s="23" t="str">
@@ -12879,7 +12879,7 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="F102" s="8"/>
       <c r="G102" s="23" t="str">
@@ -12905,7 +12905,7 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="F103" s="8"/>
       <c r="G103" s="23" t="str">
@@ -12929,7 +12929,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="F104" s="8"/>
       <c r="G104" s="23" t="str">
@@ -12951,7 +12951,7 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="F105" s="8"/>
       <c r="G105" s="23" t="str">
@@ -12974,7 +12974,7 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="F106" s="8"/>
       <c r="G106" s="23" t="str">
@@ -12996,7 +12996,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="F107" s="8"/>
       <c r="G107" s="23" t="str">
@@ -13018,7 +13018,7 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F108" s="8"/>
       <c r="G108" s="23" t="str">
@@ -13041,7 +13041,7 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="8" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="F109" s="8"/>
       <c r="G109" s="23" t="str">
@@ -13064,7 +13064,7 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="F110" s="8"/>
       <c r="G110" s="23" t="str">
@@ -13089,7 +13089,7 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="8" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="F111" s="8"/>
       <c r="G111" s="23" t="str">
@@ -13112,7 +13112,7 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="8" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="F112" s="8"/>
       <c r="G112" s="23" t="str">
@@ -13134,7 +13134,7 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="8" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="F113" s="8"/>
       <c r="G113" s="23" t="str">
@@ -13156,7 +13156,7 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="8" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="F114" s="8"/>
       <c r="G114" s="23" t="str">
@@ -13180,7 +13180,7 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="8" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="F115" s="8"/>
       <c r="G115" s="23" t="str">
@@ -13203,7 +13203,7 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="F116" s="8"/>
       <c r="G116" s="23" t="str">
@@ -13225,7 +13225,7 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="8" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="F117" s="8"/>
       <c r="G117" s="23" t="str">
@@ -13246,7 +13246,7 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="8" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="F118" s="8"/>
       <c r="G118" s="23" t="str">
@@ -13267,7 +13267,7 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="8" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="F119" s="8"/>
       <c r="G119" s="23" t="str">
@@ -13290,7 +13290,7 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="F120" s="8"/>
       <c r="G120" s="23" t="str">
@@ -13312,7 +13312,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="8" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="F121" s="8"/>
       <c r="G121" s="23" t="str">
@@ -13335,7 +13335,7 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="8" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="F122" s="8"/>
       <c r="G122" s="23" t="str">
@@ -13358,7 +13358,7 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="8" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="F123" s="8"/>
       <c r="G123" s="23" t="str">
@@ -13381,7 +13381,7 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="8" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="F124" s="8"/>
       <c r="G124" s="23" t="str">
@@ -13405,7 +13405,7 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="8" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="F125" s="8"/>
       <c r="G125" s="23" t="str">
@@ -13429,7 +13429,7 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="F126" s="8"/>
       <c r="G126" s="23" t="str">
@@ -13451,7 +13451,7 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="8" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="F127" s="8"/>
       <c r="G127" s="23" t="str">
@@ -13473,7 +13473,7 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="8" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="F128" s="8"/>
       <c r="G128" s="23" t="str">
@@ -13498,7 +13498,7 @@
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="8" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="F129" s="8"/>
       <c r="G129" s="23" t="str">
@@ -13524,7 +13524,7 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="F130" s="8"/>
       <c r="G130" s="23" t="str">
@@ -13548,7 +13548,7 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="F131" s="8"/>
       <c r="G131" s="23" t="str">
@@ -13569,7 +13569,7 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="23" t="str">
@@ -13591,7 +13591,7 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="8" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="23" t="str">
@@ -13616,7 +13616,7 @@
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="F134" s="8"/>
       <c r="G134" s="23" t="str">
@@ -13643,7 +13643,7 @@
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="23" t="str">
@@ -13722,7 +13722,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -13734,7 +13734,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix: Chapter 2 Finish Test
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2026\C++\Signal_Lost\Signal_Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6258BEFC-2CEB-49D2-8E97-B2383C83F9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4B8AFA-8005-4223-AC7D-9DB9CFD78CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters_Header" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="487">
   <si>
     <t>Chapter Name</t>
   </si>
@@ -468,12 +468,6 @@
 A bit of sunlight feels good after being in this gloomy supermarket.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Exactly what I was thinking![Wait=500][Space=2]
-Since I have no choice, let's enter slowly...[Wait=500][Space=2]
-...[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
-...[Wait=500] What is that?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>It's a flat piece of rock with engravings on it.[Wait=500][Space=2]
 It seems to be a dead language I don't know how to read.[Wait=500][Space=2]
 There is one word on here that's colored in red.[Wait=500][Space=2]
@@ -490,32 +484,9 @@
 It's the [Color=Green]"CITY NAME"[Color=White] thing, right?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Color=Gray]*BU[Beep=True]ZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
-[Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
-...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White][Wait=500] You gave me the wrong letter![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White][Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Please be right, please be right, please be right...[Wait=500][Space=2]
-[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*CLICK*[Color=White][Wait=500] The door... is unlocked![Wait=500][Space=2]
-I don't know what I'll find here, but I'm going inside anyway...[Wait=500][Space=2]
-[Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Hell-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-ou hear me?[Wait=500][Space=2]
-Why did you stop spea-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White].[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Color=Yellow]Do you think I prepared all of this for fun?[Color=White][Wait=500][Space=2]
 [Color=Yellow]I'm not some kind of sicko who likes to see 832 clones die before my eyes just for my own entertainment.[Color=White][Wait=500][Space=2]
 ...[Wait=500] 832?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>SPEAK TO M-[Color=Gray]*SHKRRRRRRRR*[Color=White].[Wait=500][Space=2]
-I don-[Color=Gray]*SHKRRRRR*[Color=White]-ear you![Wait=500][Space=2]
-[Color=Magenta][Beep=True]He[Wait=500][Beep=True] cA[Wait=500][Beep=True] n’T[Wait=500][Beep=True]  He[Wait=500][Beep=True] aR[Wait=500][Beep=True] yO[Wait=500][Beep=True] u aN[Wait=500][Beep=True] yMo[Wait=500][Beep=True] re,[Wait=500][Beep=True]  bUt[Wait=500][Beep=True]  i[Wait=500][Beep=True] cA[Wait=500][Beep=True] n He[Wait=500][Beep=True] lP[Wait=500][Beep=True] hIm.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Where should I g-[Color=Gray]*SHKRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
@@ -772,11 +743,6 @@
 The [Color=Green]"Zoo"[Color=White], the [Color=Green]"Factory"[Color=White], or the [Color=Green]"Museum"[Color=White]?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Hmmm... The buildings here look exactly the same compared to the ones I crossed before calling you...[Wait=500][Space=2]
-Hey![Wait=500] There are signs leading to two different locations here.[Wait=500][Space=2]
-One is leading to a [Color=Green]"Factory"[Color=White] and the other to a [Color=Green]"Zoo"[Color=White].[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=13][Content=Why are you doubting all of a sudden?]]
 [Choice2=[NextScene=14][NextSceneNoTrust=13][TrustNeed=50][Content=Well, you might as well go and see inside to be sure!]]</t>
   </si>
@@ -1057,12 +1023,6 @@
 I-...[Wait=500] I could do that, but nothing comes to mind that could help me escape.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I'm chicken-hearted?[Wait=500] Oh yeah?[Wait=500][Space=2]
-Well, you know what?[Wait=500] I'll enter this museum without you begging me to![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*WHAM!*[Color=White]...[Wait=500][Space=2]
-HEY![Wait=500] I JUST ENTERED YOUR MUSEUM BY KICKING THE DOOR! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>What did I hear?[Wait=500] Is someone getting scared all of a sudden?[Wait=500] That’ll teach you![Wait=500][Space=2]
 But there doesn’t seem to be anyone here anyway.[Wait=500][Space=2]
 Looks like we both worried for nothing.[Wait=500][Space=2]
@@ -1083,11 +1043,6 @@
 I don’t want to end up face-to-face with someone hostile.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>If I were to listen to myself, I wouldn’t enter this place because it freaks me out for some reason...[Wait=500][Space=2]
-But you’re here! I’ve got nothing to be afraid of, so I’m heading inside![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>The inside of this museum truly feels abnormal...[Wait=500][Space=2]
 Everything’s clean. There’s not a single bit of dust here![Wait=500][Space=2]
 All these paintings are perfectly displayed,[Wait=500] the sculptures are brightly polished...[Wait=500][Space=2]
@@ -1129,20 +1084,9 @@
 Now, this philosophical question is interesting, but it won't help me escape from here, so let's explore this place![Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Ah![Wait=500] You act all confident, but you couldn’t handle a quarter of what I’m going through![Wait=500][Space=2]
-...[Wait=500] I’m the one making fun of you, but in the end, I’m still the one stuck on this island...[Wait=500] Ironic.[Wait=500][Space=2]
-It might be the right time to come back to the main question: what is this place?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Phew...[Wait=500] That’s true.[Wait=500][Space=2]
 I’m not in imminent danger...[Wait=500] I just need to focus on my escape and everything will be okay![Wait=500][Space=2]
 I needed to reassure myself before doing a bit of exploration, sorry.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White][Wait=500] I don’t care about the art![Wait=500][Space=2]
-You know it’s really not the time to be joking around, right?[Wait=500][Space=2]
-I’m diving into the unknown and you think it’s funny?[Wait=500] That’s really irritating![Wait=500][Space=2]
-I don’t want to argue here, so let’s go see what this museum has to offer.[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Well, I hope you’re not a comedian![Wait=500][Space=2]
@@ -1168,11 +1112,6 @@
 Too bad I can’t speak that language though.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I thought the same thing...[Wait=500] I’m not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
-I’m here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
-[Color=Gray]*CRACK*[Color=White][Wait=500] Shit, I didn’t know kicking a statue could dislocate its leg—[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I-I don’t know, the ground shook for a second...[Wait=500][Space=2]
 Wait...[Wait=500] What’s tha-...[Wait=500][Space=2]
 ...Did a motherfucking door just appear at the back of the museum?![Wait=500][Space=2]
@@ -1215,19 +1154,6 @@
   <si>
     <t>Are you sure?[Wait=500] I don't know what could happen if I type the wrong code, but I don't want to find out.[Wait=500][Space=2]
 You're confident?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] I'm shaking with fear, but I need to concentrate to click on the right button...[Wait=500][Space=2]
-[Color=Gray]*B[Beep=True]#eep*[Color=White]...[Wait=500][Space=2]
-Oh yes! It didn't explode or anything, so we may be on the right path![Wait=500][Space=2]
-The second letter was [Color=Green]"ARTIST NAME"[Color=White].[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
-I c...[Wait=500] [Color=Gray]*Cough*[Color=White][Wait=500] I can't breathe![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
-Arhh...[Wait=500][Space=2]
-...[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>...[Wait=500][Space=2]
@@ -1282,19 +1208,6 @@
 It's too late to change my mind.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
-There are multiple corridors leading to-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] I don't know which one is the right one![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Magenta][Beep=True]Th[Wait=500][Beep=True] aT[Wait=500][Beep=True] wI[Wait=500][Beep=True] lL dO[Wait=500][Beep=True]... Th[Wait=500][Beep=True] aNkS fO[Wait=500][Beep=True] r Y[Wait=500][Beep=True] oU r H[Wait=500][Beep=True] eLp.[Color=White][Wait=500][Space=2]
-...[Color=Gray]*SHKRRRR*[Color=White] Hello?[Wait=500] Hey?[Wait=500][Space=2]
-Can you hear me?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Yeah, as if you could pretend that![Wait=500][Space=2]
-Anyway, let's focus on the most important question: WHO WAS THAT?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Are you serious...[Wait=500][Space=2]
 You know what? Forget it...[Wait=500] The most important thing is who the hell was this person asking you all this?[Wait=500][Space=2]</t>
   </si>
@@ -1303,12 +1216,6 @@
 The more I realize the situation I'm in, the less I think all of this makes sense...[Wait=500][Space=2]
 Anyway, I'm inside a complex of whitish corridors, the-[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
 Wait...[Wait=500] Those footsteps weren't mine...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White] It's getting closer![Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
-[Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
     <t>[Color=Yellow]No matter what your friend says, it's just between me and you, subject 835...[Color=White][Wait=500][Space=2]
@@ -1366,20 +1273,6 @@
 [Color=Yellow]...[Wait=500] Hmmm...[Wait=500] Unfortunately for you, I anticipated this kind of reaction.[Color=White][Wait=500][Space=2]
 [Color=Yellow]What are your last words?[Color=White][Wait=500][Space=2]
 Y-You're bluffing![Wait=500] I'm not going to fall for this eith-[Color=Gray]*PSHHHHHHHHHH*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] OH SHIT![Wait=500] THERE'S GREEN GAS SPREADING IN THE ROOM![Wait=500][Space=2]
-[Color=Gray]*Door shake*[Color=White]...[Wait=500][Space=2]
-LET ME OUT, THIS FUCKER LOCKED THE DOOR![Wait=500][Space=2]
-[Color=Yellow]You made your own choices, you and your friend.[Wait=500] Now you'll have to accept the consequences.[Color=White][Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White] [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
-.[Wait=500].[Wait=500].[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
-I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beginning, right?[Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White] OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
-[Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>LIAR![Wait=500][Space=2]
@@ -1909,15 +1802,6 @@
 [Color=Magenta][Beep=True]Fi[Wait=500][Beep=True]nD tHe[Wait=500][Beep=True]  cO[Wait=500][Beep=True]dE.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>It says:[Wait=500][Space=2]
-[Color=Green]"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
--FIRST LETTER = CITY NAME.[Wait=500][Space=2]
--SECOND LETTER = ARTIST NAME.[Wait=500][Space=2]
--THIRD LETTER = TRANSLATED IN ENGLISH.[Wait=500][Space=2]
-KEEP EVERYONE OUT AT ALL COSTS."[Color=White]...[Wait=500][Space=2]
-...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>What do you mean a co-...[Wait=500] Huh?[Wait=500][Space=2]
 There are inscriptions on the wall...[Wait=500] It says:[Wait=500][Space=2]
 [Color=Green]"MK BLOOD CODE:[Wait=500][Space=2]
@@ -2466,6 +2350,126 @@
 HNNG![Wait=500] Huff...[Wait=500] I can't open it with my bare hands either.[Wait=500][Space=2]
 It seems locked by some kind of electrical mechanism that leads to this control panel.[Wait=500][Space=2]
 ...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Hmmm...[Wait=500] The buildings here look exactly the same compared to the ones I crossed before calling you...[Wait=500][Space=2]
+Hey![Wait=500] There are signs leading to two different locations here.[Wait=500][Space=2]
+One is leading to a [Color=Green]"Factory"[Color=White] and the other to a [Color=Green]"Zoo"[Color=White].[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Exactly what I was thinking![Wait=500][Space=2]
+Since I have no choice, let's enter slowly...[Wait=500][Space=2]
+...[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
+...[Wait=500] What is that?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm chicken-hearted?[Wait=500] Oh yeah?[Wait=500][Space=2]
+Well, you know what?[Wait=500] I'll enter this museum without you begging me to![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*WHAM!*[Color=White]...[Wait=500][Space=2]
+HEY![Wait=500] I JUST ENTERED YOUR MUSEUM BY KICKING THE DOOR! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>If I were to listen to myself, I wouldn’t enter this place because it freaks me out for some reason...[Wait=500][Space=2]
+But you’re here! I’ve got nothing to be afraid of, so I’m heading inside![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ah![Wait=500] You act all confident, but you couldn’t handle a quarter of what I’m going through![Wait=500][Space=2]
+...[Wait=500] I’m the one making fun of you, but in the end, I’m still the one stuck on this island...[Wait=500] Ironic.[Wait=500][Space=2]
+It might be the right time to come back to the main question,[Wait=500] what is this place?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White]...[Wait=500] I don’t care about the art![Wait=500][Space=2]
+You know it’s really not the time to be joking around, right?[Wait=500][Space=2]
+I’m diving into the unknown and you think it’s funny?[Wait=500] That’s really irritating![Wait=500][Space=2]
+I don’t want to argue here, so let’s go see what this museum has to offer.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I thought the same thing...[Wait=500] I’m not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
+I’m here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
+[Color=Gray]*CRACK*[Color=White]...[Wait=500] Shit, I didn’t know kicking a statue could dislocate its leg—[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It says:[Wait=500][Space=2]
+"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
+[Color=Green]-FIRST LETTER = CITY NAME.[Wait=500][Space=2]
+-SECOND LETTER = ARTIST NAME.[Wait=500][Space=2]
+-THIRD LETTER = TRANSLATED IN ENGLISH.[Color=White][Wait=500][Space=2]
+KEEP EVERYONE OUT AT ALL COSTS."...[Wait=500][Space=2]
+...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It’s a really good-looking rock, with good-looking inscriptions on it![Wait=500][Space=2]
+Too bad, I can’t speak that language though.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] I'm shaking with fear, but I need to concentrate to click on the right button...[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
+Oh yes! It didn't explode or anything, so we may be on the right path![Wait=500][Space=2]
+The second letter was [Color=Green]"ARTIST NAME"[Color=White].[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
+[Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
+...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] You gave me the wrong letter![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+I c...[Wait=500] [Color=Gray]*Cough*[Color=White]...[Wait=500] I can't breathe![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+Arhh...[Wait=500][Space=2]
+...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Please be right, please be right, please be right...[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*CLICK*[Color=White]...[Wait=500] The door... is unlocked![Wait=500][Space=2]
+I don't know what I'll find here, but I'm going inside anyway...[Wait=500][Space=2]
+[Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+There are multiple corridors leading to-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] I don't know which one is the right one![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Hell-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-ou hear me?[Wait=500][Space=2]
+Why did you stop spea-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>SPEAK TO M-[Color=Gray]*SHKRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+I don-[Color=Gray]*SHKRRRRR*[Color=White]-ear you![Wait=500][Space=2]
+[Color=Magenta][Beep=True]He[Wait=500][Beep=True] cA[Wait=500][Beep=True] n’T[Wait=500][Beep=True]  He[Wait=500][Beep=True] aR[Wait=500][Beep=True] yO[Wait=500][Beep=True] u aN[Wait=500][Beep=True] yMo[Wait=500][Beep=True] re,[Wait=500][Beep=True]  bUt[Wait=500][Beep=True]  i[Wait=500][Beep=True] cA[Wait=500][Beep=True] n He[Wait=500][Beep=True] lP[Wait=500][Beep=True] hIm.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Magenta][Beep=True]Th[Wait=500][Beep=True] aT[Wait=500][Beep=True] wI[Wait=500][Beep=True] lL dO[Wait=500][Beep=True]... Th[Wait=500][Beep=True] aNkS fO[Wait=500][Beep=True] r Y[Wait=500][Beep=True] oU r H[Wait=500][Beep=True] eLp.[Color=White][Wait=500][Space=2]
+...[Color=Gray]*SHKRRRR*[Color=White]-Hello?[Wait=500] Hey?[Wait=500][Space=2]
+Can you hear me?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah, as if you could pretend that![Wait=500][Space=2]
+Anyway, let's focus on the most important question.[Wait=500] WHO WAS THAT?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's getting closer![Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
+I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
+[Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] OH SHIT![Wait=500] THERE'S GREEN GAS SPREADING IN THE ROOM![Wait=500][Space=2]
+[Color=Gray]*Door shake*[Color=White]...[Wait=500][Space=2]
+LET ME OUT, THIS FUCKER LOCKED THE DOOR![Wait=500][Space=2]
+[Color=Yellow]You made your own choices, you and your friend.[Wait=500] Now you'll have to accept the consequences.[Color=White][Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White]... [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
+I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beginning, right?[Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White]... OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
+[Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]</t>
   </si>
 </sst>
 </file>
@@ -4983,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="C2" s="12">
         <v>4</v>
@@ -5099,8 +5103,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView topLeftCell="B72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5121,7 +5125,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -5133,7 +5137,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5150,7 +5154,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>26</v>
@@ -5180,7 +5184,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
@@ -5211,10 +5215,10 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5243,7 +5247,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>23</v>
@@ -5270,7 +5274,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>24</v>
@@ -5330,7 +5334,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>30</v>
@@ -5387,7 +5391,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>29</v>
@@ -5417,10 +5421,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5446,7 +5450,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>31</v>
@@ -5506,7 +5510,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5530,7 +5534,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>33</v>
@@ -5587,7 +5591,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>34</v>
@@ -5619,7 +5623,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5731,7 +5735,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>49</v>
@@ -5763,7 +5767,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>50</v>
@@ -5796,10 +5800,10 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5861,10 +5865,10 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5893,7 +5897,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>38</v>
@@ -5920,7 +5924,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>39</v>
@@ -5947,7 +5951,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>51</v>
@@ -5977,7 +5981,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>52</v>
@@ -6093,7 +6097,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>56</v>
@@ -6123,7 +6127,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>57</v>
@@ -6187,7 +6191,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>59</v>
@@ -6220,7 +6224,7 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>60</v>
@@ -6251,7 +6255,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>40</v>
@@ -6279,7 +6283,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>61</v>
@@ -6308,7 +6312,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>62</v>
@@ -6337,7 +6341,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>63</v>
@@ -6367,7 +6371,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>41</v>
@@ -6396,7 +6400,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>41</v>
@@ -6424,7 +6428,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>42</v>
@@ -6453,7 +6457,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>64</v>
@@ -6481,7 +6485,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>65</v>
@@ -6509,7 +6513,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>66</v>
@@ -6537,7 +6541,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>67</v>
@@ -6566,7 +6570,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>68</v>
@@ -6594,7 +6598,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>43</v>
@@ -6623,7 +6627,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>69</v>
@@ -6693,7 +6697,7 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>45</v>
@@ -6722,10 +6726,10 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6787,7 +6791,7 @@
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>70</v>
@@ -6872,7 +6876,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>72</v>
@@ -6900,7 +6904,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>73</v>
@@ -6927,7 +6931,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>48</v>
@@ -6955,7 +6959,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>74</v>
@@ -6983,7 +6987,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>75</v>
@@ -7012,7 +7016,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>76</v>
@@ -7038,7 +7042,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>77</v>
@@ -7095,7 +7099,7 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>79</v>
@@ -7126,7 +7130,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>80</v>
@@ -7155,7 +7159,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>81</v>
@@ -7184,7 +7188,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>83</v>
@@ -7211,7 +7215,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>82</v>
@@ -7243,7 +7247,7 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>162</v>
+        <v>466</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>84</v>
@@ -7253,7 +7257,7 @@
         <v>[Scene=72
 [Connection=3]
 [Content=
-Hmmm... The buildings here look exactly the same compared to the ones I crossed before calling you...[Wait=500][Space=2]
+Hmmm...[Wait=500] The buildings here look exactly the same compared to the ones I crossed before calling you...[Wait=500][Space=2]
 Hey![Wait=500] There are signs leading to two different locations here.[Wait=500][Space=2]
 One is leading to a [Color=Green]"Factory"[Color=White] and the other to a [Color=Green]"Zoo"[Color=White].[Wait=500][Space=2]
 ]
@@ -7329,8 +7333,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView topLeftCell="B53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7351,7 +7355,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -7363,7 +7367,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7376,10 +7380,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -7403,10 +7407,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7435,7 +7439,7 @@
         <v>91</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7459,10 +7463,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7488,10 +7492,10 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7516,10 +7520,10 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7543,10 +7547,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7570,10 +7574,10 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>105</v>
+        <v>467</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7581,7 +7585,7 @@
 [Content=
 Exactly what I was thinking![Wait=500][Space=2]
 Since I have no choice, let's enter slowly...[Wait=500][Space=2]
-...[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
+...[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500] What is that?[Wait=500][Space=2]
 ]
 [Choices=
@@ -7598,10 +7602,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>235</v>
+        <v>468</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7609,7 +7613,7 @@
 [Content=
 I'm chicken-hearted?[Wait=500] Oh yeah?[Wait=500][Space=2]
 Well, you know what?[Wait=500] I'll enter this museum without you begging me to![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*WHAM!*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*WHAM!*[Color=White]...[Wait=500][Space=2]
 HEY![Wait=500] I JUST ENTERED YOUR MUSEUM BY KICKING THE DOOR! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]
 ]
 [Choices=
@@ -7627,10 +7631,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7655,10 +7659,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7682,10 +7686,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7709,10 +7713,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7737,10 +7741,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>240</v>
+        <v>469</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7748,7 +7752,7 @@
 [Content=
 If I were to listen to myself, I wouldn’t enter this place because it freaks me out for some reason...[Wait=500][Space=2]
 But you’re here! I’ve got nothing to be afraid of, so I’m heading inside![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=15][Content=So? What’s inside?]]
@@ -7764,10 +7768,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7793,10 +7797,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7822,10 +7826,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7851,10 +7855,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7880,10 +7884,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7909,10 +7913,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7936,10 +7940,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7964,10 +7968,10 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -7990,10 +7994,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>249</v>
+        <v>470</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8001,7 +8005,7 @@
 [Content=
 Ah![Wait=500] You act all confident, but you couldn’t handle a quarter of what I’m going through![Wait=500][Space=2]
 ...[Wait=500] I’m the one making fun of you, but in the end, I’m still the one stuck on this island...[Wait=500] Ironic.[Wait=500][Space=2]
-It might be the right time to come back to the main question: what is this place?[Wait=500][Space=2]
+It might be the right time to come back to the main question,[Wait=500] what is this place?[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=27][Content=What’s around you again?]]
@@ -8017,10 +8021,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8044,16 +8048,16 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>251</v>
+        <v>471</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=25
 [Content=
-Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White][Wait=500] I don’t care about the art![Wait=500][Space=2]
+Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White]...[Wait=500] I don’t care about the art![Wait=500][Space=2]
 You know it’s really not the time to be joking around, right?[Wait=500][Space=2]
 I’m diving into the unknown and you think it’s funny?[Wait=500] That’s really irritating![Wait=500][Space=2]
 I don’t want to argue here, so let’s go see what this museum has to offer.[Wait=500][Space=2]
@@ -8072,10 +8076,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8100,10 +8104,10 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8129,10 +8133,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8156,10 +8160,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8183,10 +8187,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8210,10 +8214,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>257</v>
+        <v>472</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8221,7 +8225,7 @@
 [Content=
 I thought the same thing...[Wait=500] I’m not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
 I’m here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
-[Color=Gray]*CRACK*[Color=White][Wait=500] Shit, I didn’t know kicking a statue could dislocate its leg—[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]
+[Color=Gray]*CRACK*[Color=White]...[Wait=500] Shit, I didn’t know kicking a statue could dislocate its leg—[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=32][Content=What’s going on?]]
@@ -8237,10 +8241,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8266,10 +8270,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -8294,21 +8298,21 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>392</v>
+        <v>473</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=34
 [Content=
 It says:[Wait=500][Space=2]
-[Color=Green]"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
--FIRST LETTER = CITY NAME.[Wait=500][Space=2]
+"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
+[Color=Green]-FIRST LETTER = CITY NAME.[Wait=500][Space=2]
 -SECOND LETTER = ARTIST NAME.[Wait=500][Space=2]
--THIRD LETTER = TRANSLATED IN ENGLISH.[Wait=500][Space=2]
-KEEP EVERYONE OUT AT ALL COSTS."[Color=White]...[Wait=500][Space=2]
+-THIRD LETTER = TRANSLATED IN ENGLISH.[Color=White][Wait=500][Space=2]
+KEEP EVERYONE OUT AT ALL COSTS."...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
 [Choices=
@@ -8326,10 +8330,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8357,10 +8361,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8383,10 +8387,10 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8409,17 +8413,17 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>256</v>
+        <v>474</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=38
 [Content=
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] It’s a really good-looking rock, with good-looking inscriptions on it![Wait=500][Space=2]
-Too bad I can’t speak that language though.[Wait=500][Space=2]
+Too bad, I can’t speak that language though.[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=44][Content=Can I have more information about it?]]
@@ -8435,10 +8439,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8462,10 +8466,10 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8490,10 +8494,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8518,10 +8522,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8545,10 +8549,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8573,10 +8577,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8601,10 +8605,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8628,10 +8632,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8658,17 +8662,17 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>266</v>
+        <v>475</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=47
 [Content=
 ...[Wait=500] I'm shaking with fear, but I need to concentrate to click on the right button...[Wait=500][Space=2]
-[Color=Gray]*B[Beep=True]#eep*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
 Oh yes! It didn't explode or anything, so we may be on the right path![Wait=500][Space=2]
 The second letter was [Color=Green]"ARTIST NAME"[Color=White].[Wait=500][Space=2]
 ]
@@ -8690,10 +8694,10 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8724,21 +8728,21 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>109</v>
+        <v>476</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=49
 [Connection=2]
 [Content=
-[Color=Gray]*BU[Beep=True]ZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
 [Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
 ...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White][Wait=500] You gave me the wrong letter![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White][Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] You gave me the wrong letter![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=50][Content=You have to get out!]]
@@ -8756,19 +8760,19 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>267</v>
+        <v>477</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=50
 [Connection=1]
 [Content=
-[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
-I c...[Wait=500] [Color=Gray]*Cough*[Color=White][Wait=500] I can't breathe![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+I c...[Wait=500] [Color=Gray]*Cough*[Color=White]...[Wait=500] I can't breathe![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
 Arhh...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
@@ -8788,10 +8792,10 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8820,10 +8824,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>110</v>
+        <v>478</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8831,7 +8835,7 @@
 [Content=
 Please be right, please be right, please be right...[Wait=500][Space=2]
 [Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*CLICK*[Color=White][Wait=500] The door... is unlocked![Wait=500][Space=2]
+[Color=Gray]*CLICK*[Color=White]...[Wait=500] The door... is unlocked![Wait=500][Space=2]
 I don't know what I'll find here, but I'm going inside anyway...[Wait=500][Space=2]
 [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]
 ]
@@ -8849,10 +8853,10 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8878,10 +8882,10 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8907,10 +8911,10 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8934,10 +8938,10 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8960,10 +8964,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
@@ -8986,10 +8990,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9017,7 +9021,7 @@
         <v>95</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9041,10 +9045,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9072,7 +9076,7 @@
         <v>96</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9096,10 +9100,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9126,7 +9130,7 @@
         <v>97</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9151,17 +9155,17 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>278</v>
+        <v>479</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=64
 [Connection=2]
 [Content=
-I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
+I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 There are multiple corridors leading to-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] I don't know which one is the right one![Wait=500][Space=2]
 ]
 [Choices=
@@ -9180,10 +9184,10 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>111</v>
+        <v>480</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G97" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -9191,7 +9195,7 @@
 [Connection=1]
 [Content=
 Hell-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-ou hear me?[Wait=500][Space=2]
-Why did you stop spea-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
+Why did you stop spea-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=66][Content=Can you hear me?]]
@@ -9208,16 +9212,16 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>113</v>
+        <v>481</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=66
 [Content=
-SPEAK TO M-[Color=Gray]*SHKRRRRRRRR*[Color=White].[Wait=500][Space=2]
+SPEAK TO M-[Color=Gray]*SHKRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 I don-[Color=Gray]*SHKRRRRR*[Color=White]-ear you![Wait=500][Space=2]
 [Color=Magenta][Beep=True]He[Wait=500][Beep=True] cA[Wait=500][Beep=True] n’T[Wait=500][Beep=True]  He[Wait=500][Beep=True] aR[Wait=500][Beep=True] yO[Wait=500][Beep=True] u aN[Wait=500][Beep=True] yMo[Wait=500][Beep=True] re,[Wait=500][Beep=True]  bUt[Wait=500][Beep=True]  i[Wait=500][Beep=True] cA[Wait=500][Beep=True] n He[Wait=500][Beep=True] lP[Wait=500][Beep=True] hIm.[Color=White][Wait=500][Space=2]
 ]
@@ -9235,10 +9239,10 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9262,10 +9266,10 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9289,10 +9293,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9318,10 +9322,10 @@
         <v>7</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9348,10 +9352,10 @@
         <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9378,10 +9382,10 @@
         <v>7</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9406,17 +9410,17 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="8" t="s">
-        <v>279</v>
+        <v>482</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G74" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=73
 [Content=
 [Color=Magenta][Beep=True]Th[Wait=500][Beep=True] aT[Wait=500][Beep=True] wI[Wait=500][Beep=True] lL dO[Wait=500][Beep=True]... Th[Wait=500][Beep=True] aNkS fO[Wait=500][Beep=True] r Y[Wait=500][Beep=True] oU r H[Wait=500][Beep=True] eLp.[Color=White][Wait=500][Space=2]
-...[Color=Gray]*SHKRRRR*[Color=White] Hello?[Wait=500] Hey?[Wait=500][Space=2]
+...[Color=Gray]*SHKRRRR*[Color=White]-Hello?[Wait=500] Hey?[Wait=500][Space=2]
 Can you hear me?[Wait=500][Space=2]
 ]
 [Choices=
@@ -9439,7 +9443,7 @@
         <v>99</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G75" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9467,7 +9471,7 @@
         <v>98</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G76" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9490,17 +9494,17 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>280</v>
+        <v>483</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G77" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=76
 [Content=
 Yeah, as if you could pretend that![Wait=500][Space=2]
-Anyway, let's focus on the most important question: WHO WAS THAT?[Wait=500][Space=2]
+Anyway, let's focus on the most important question.[Wait=500] WHO WAS THAT?[Wait=500][Space=2]
 ]
 [Choices=
 [Choice1=[NextScene=78][Content=I have no idea!]]
@@ -9516,10 +9520,10 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G78" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9542,10 +9546,10 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G79" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9570,16 +9574,16 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>283</v>
+        <v>484</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G80" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=79
 [Content=
-[Color=Gray]*Footsteps*[Color=White] It's getting closer![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's getting closer![Wait=500][Space=2]
 [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
 I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
 [Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]
@@ -9599,10 +9603,10 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G81" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9627,10 +9631,10 @@
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G82" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9655,10 +9659,10 @@
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="8" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G83" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9682,10 +9686,10 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G84" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9709,10 +9713,10 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G85" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9736,10 +9740,10 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G86" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9765,10 +9769,10 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G87" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9793,10 +9797,10 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9821,10 +9825,10 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G89" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9849,10 +9853,10 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G90" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9880,10 +9884,10 @@
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="G91" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9912,10 +9916,10 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8" t="s">
-        <v>294</v>
+        <v>485</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="G92" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9926,7 +9930,7 @@
 [Color=Gray]*Door shake*[Color=White]...[Wait=500][Space=2]
 LET ME OUT, THIS FUCKER LOCKED THE DOOR![Wait=500][Space=2]
 [Color=Yellow]You made your own choices, you and your friend.[Wait=500] Now you'll have to accept the consequences.[Color=White][Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White] [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White]... [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
 .[Wait=500].[Wait=500].[Wait=500][Space=2]
 ]
 [Choices=
@@ -9945,10 +9949,10 @@
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G93" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9981,10 +9985,10 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8" t="s">
-        <v>295</v>
+        <v>486</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G94" s="23" t="str">
         <f t="shared" si="2"/>
@@ -9993,7 +9997,7 @@
 [Content=
 N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
 I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beginning, right?[Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White] OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White]... OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
 [Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]
 ]
 [Choices=
@@ -10011,10 +10015,10 @@
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G95" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10037,10 +10041,10 @@
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G96" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10067,10 +10071,10 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G97" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10096,10 +10100,10 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G98" s="23" t="str">
         <f t="shared" ref="G98:G108" si="3">"[Scene=" &amp; A98 &amp; IF(OR(B98&lt;&gt;"",C98&lt;&gt;"",D98&lt;&gt;""),CHAR(10),"") &amp; IF(B98&lt;&gt;"","[BeepBack=" &amp; B98 &amp; "]","") &amp; IF(C98&lt;&gt;"","[Connection=" &amp; C98 &amp; "]","") &amp; IF(D98&lt;&gt;"","[Timer=" &amp; D98 &amp; "]","") &amp; IF(E98&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E98 &amp; CHAR(10) &amp; "]","") &amp; IF(F98&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F98 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -10127,10 +10131,10 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G99" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10158,10 +10162,10 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10192,10 +10196,10 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G101" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10223,10 +10227,10 @@
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G102" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10255,10 +10259,10 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G103" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10287,10 +10291,10 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G104" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10316,10 +10320,10 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G105" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10344,10 +10348,10 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10373,10 +10377,10 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G107" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10403,10 +10407,10 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G108" s="24" t="str">
         <f t="shared" si="3"/>
@@ -10490,7 +10494,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -10502,7 +10506,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10515,7 +10519,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="23" t="str">
@@ -10538,7 +10542,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="23" t="str">
@@ -10561,7 +10565,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="23" t="str">
@@ -10582,7 +10586,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="23" t="str">
@@ -10606,7 +10610,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="23" t="str">
@@ -10629,7 +10633,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="23" t="str">
@@ -10653,7 +10657,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="23" t="str">
@@ -10678,7 +10682,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="23" t="str">
@@ -10702,7 +10706,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="23" t="str">
@@ -10727,7 +10731,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="23" t="str">
@@ -10749,7 +10753,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="23" t="str">
@@ -10772,7 +10776,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="23" t="str">
@@ -10794,7 +10798,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="23" t="str">
@@ -10816,7 +10820,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="23" t="str">
@@ -10837,7 +10841,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="23" t="str">
@@ -10862,7 +10866,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="23" t="str">
@@ -10887,7 +10891,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="23" t="str">
@@ -10911,7 +10915,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="23" t="str">
@@ -10932,7 +10936,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="23" t="str">
@@ -10955,7 +10959,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="23" t="str">
@@ -10976,7 +10980,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="23" t="str">
@@ -10998,7 +11002,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="23" t="str">
@@ -11021,7 +11025,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="23" t="str">
@@ -11045,7 +11049,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="23" t="str">
@@ -11069,7 +11073,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="23" t="str">
@@ -11094,7 +11098,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="23" t="str">
@@ -11117,7 +11121,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="23" t="str">
@@ -11140,7 +11144,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="23" t="str">
@@ -11163,7 +11167,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="23" t="str">
@@ -11187,7 +11191,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="23" t="str">
@@ -11210,7 +11214,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="23" t="str">
@@ -11233,7 +11237,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="23" t="str">
@@ -11255,7 +11259,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="23" t="str">
@@ -11278,7 +11282,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="23" t="str">
@@ -11300,7 +11304,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="23" t="str">
@@ -11324,7 +11328,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="23" t="str">
@@ -11347,7 +11351,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="23" t="str">
@@ -11373,7 +11377,7 @@
         <v>60</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="23" t="str">
@@ -11399,7 +11403,7 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="23" t="str">
@@ -11427,7 +11431,7 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="23" t="str">
@@ -11456,7 +11460,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="23" t="str">
@@ -11482,7 +11486,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="23" t="str">
@@ -11504,7 +11508,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="23" t="str">
@@ -11527,7 +11531,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="23" t="str">
@@ -11550,7 +11554,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="23" t="str">
@@ -11572,7 +11576,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="23" t="str">
@@ -11596,7 +11600,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="23" t="str">
@@ -11618,7 +11622,7 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="23" t="str">
@@ -11646,7 +11650,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="23" t="str">
@@ -11669,7 +11673,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="23" t="str">
@@ -11690,7 +11694,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="23" t="str">
@@ -11713,7 +11717,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="23" t="str">
@@ -11737,7 +11741,7 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="23" t="str">
@@ -11759,7 +11763,7 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="23" t="str">
@@ -11781,7 +11785,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="23" t="str">
@@ -11803,7 +11807,7 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="23" t="str">
@@ -11825,7 +11829,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="23" t="str">
@@ -11847,7 +11851,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="23" t="str">
@@ -11873,7 +11877,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="23" t="str">
@@ -11895,7 +11899,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="23" t="str">
@@ -11916,7 +11920,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="23" t="str">
@@ -11939,7 +11943,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="23" t="str">
@@ -11961,7 +11965,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="23" t="str">
@@ -11982,7 +11986,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="23" t="str">
@@ -12007,7 +12011,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="23" t="str">
@@ -12034,7 +12038,7 @@
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="23" t="str">
@@ -12061,7 +12065,7 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="23" t="str">
@@ -12087,7 +12091,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="23" t="str">
@@ -12110,7 +12114,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="23" t="str">
@@ -12132,7 +12136,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="23" t="str">
@@ -12156,7 +12160,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="23" t="str">
@@ -12179,7 +12183,7 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="F73" s="8"/>
       <c r="G73" s="23" t="str">
@@ -12202,7 +12206,7 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="F74" s="13"/>
       <c r="G74" s="24" t="str">
@@ -12225,7 +12229,7 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="23" t="str">
@@ -12246,7 +12250,7 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="23" t="str">
@@ -12268,7 +12272,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="23" t="str">
@@ -12291,7 +12295,7 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="23" t="str">
@@ -12313,7 +12317,7 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="23" t="str">
@@ -12336,7 +12340,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="23" t="str">
@@ -12359,7 +12363,7 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="23" t="str">
@@ -12384,7 +12388,7 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="23" t="str">
@@ -12410,7 +12414,7 @@
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="24" t="str">
@@ -12437,7 +12441,7 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="F84" s="8"/>
       <c r="G84" s="23" t="str">
@@ -12461,7 +12465,7 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
       <c r="F85" s="8"/>
       <c r="G85" s="23" t="str">
@@ -12483,7 +12487,7 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="F86" s="8"/>
       <c r="G86" s="23" t="str">
@@ -12505,7 +12509,7 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="F87" s="8"/>
       <c r="G87" s="23" t="str">
@@ -12527,7 +12531,7 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="23" t="str">
@@ -12550,7 +12554,7 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="F89" s="8"/>
       <c r="G89" s="23" t="str">
@@ -12572,7 +12576,7 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="23" t="str">
@@ -12595,7 +12599,7 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="23" t="str">
@@ -12619,7 +12623,7 @@
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="24" t="str">
@@ -12647,7 +12651,7 @@
         <v>10</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="F93" s="8"/>
       <c r="G93" s="23" t="str">
@@ -12673,7 +12677,7 @@
         <v>10</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="F94" s="8"/>
       <c r="G94" s="23" t="str">
@@ -12698,7 +12702,7 @@
         <v>10</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="F95" s="8"/>
       <c r="G95" s="23" t="str">
@@ -12725,7 +12729,7 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
       <c r="F96" s="8"/>
       <c r="G96" s="23" t="str">
@@ -12750,7 +12754,7 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="F97" s="8"/>
       <c r="G97" s="23" t="str">
@@ -12775,7 +12779,7 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="F98" s="8"/>
       <c r="G98" s="23" t="str">
@@ -12800,7 +12804,7 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="F99" s="8"/>
       <c r="G99" s="23" t="str">
@@ -12826,7 +12830,7 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="F100" s="8"/>
       <c r="G100" s="23" t="str">
@@ -12852,7 +12856,7 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="F101" s="8"/>
       <c r="G101" s="23" t="str">
@@ -12879,7 +12883,7 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="F102" s="8"/>
       <c r="G102" s="23" t="str">
@@ -12905,7 +12909,7 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
       <c r="F103" s="8"/>
       <c r="G103" s="23" t="str">
@@ -12929,7 +12933,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="F104" s="8"/>
       <c r="G104" s="23" t="str">
@@ -12951,7 +12955,7 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="F105" s="8"/>
       <c r="G105" s="23" t="str">
@@ -12974,7 +12978,7 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="F106" s="8"/>
       <c r="G106" s="23" t="str">
@@ -12996,7 +13000,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="F107" s="8"/>
       <c r="G107" s="23" t="str">
@@ -13018,7 +13022,7 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="F108" s="8"/>
       <c r="G108" s="23" t="str">
@@ -13041,7 +13045,7 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="8" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="F109" s="8"/>
       <c r="G109" s="23" t="str">
@@ -13064,7 +13068,7 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="F110" s="8"/>
       <c r="G110" s="23" t="str">
@@ -13089,7 +13093,7 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="8" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="F111" s="8"/>
       <c r="G111" s="23" t="str">
@@ -13112,7 +13116,7 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="8" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="F112" s="8"/>
       <c r="G112" s="23" t="str">
@@ -13134,7 +13138,7 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="8" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="F113" s="8"/>
       <c r="G113" s="23" t="str">
@@ -13156,7 +13160,7 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="8" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="F114" s="8"/>
       <c r="G114" s="23" t="str">
@@ -13180,7 +13184,7 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="8" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="F115" s="8"/>
       <c r="G115" s="23" t="str">
@@ -13203,7 +13207,7 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="F116" s="8"/>
       <c r="G116" s="23" t="str">
@@ -13225,7 +13229,7 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="8" t="s">
-        <v>451</v>
+        <v>431</v>
       </c>
       <c r="F117" s="8"/>
       <c r="G117" s="23" t="str">
@@ -13246,7 +13250,7 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="8" t="s">
-        <v>452</v>
+        <v>432</v>
       </c>
       <c r="F118" s="8"/>
       <c r="G118" s="23" t="str">
@@ -13267,7 +13271,7 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="8" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
       <c r="F119" s="8"/>
       <c r="G119" s="23" t="str">
@@ -13290,7 +13294,7 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="8" t="s">
-        <v>455</v>
+        <v>435</v>
       </c>
       <c r="F120" s="8"/>
       <c r="G120" s="23" t="str">
@@ -13312,7 +13316,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="8" t="s">
-        <v>456</v>
+        <v>436</v>
       </c>
       <c r="F121" s="8"/>
       <c r="G121" s="23" t="str">
@@ -13335,7 +13339,7 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="8" t="s">
-        <v>457</v>
+        <v>437</v>
       </c>
       <c r="F122" s="8"/>
       <c r="G122" s="23" t="str">
@@ -13358,7 +13362,7 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="8" t="s">
-        <v>458</v>
+        <v>438</v>
       </c>
       <c r="F123" s="8"/>
       <c r="G123" s="23" t="str">
@@ -13381,7 +13385,7 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="8" t="s">
-        <v>459</v>
+        <v>439</v>
       </c>
       <c r="F124" s="8"/>
       <c r="G124" s="23" t="str">
@@ -13405,7 +13409,7 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="8" t="s">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="F125" s="8"/>
       <c r="G125" s="23" t="str">
@@ -13429,7 +13433,7 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="F126" s="8"/>
       <c r="G126" s="23" t="str">
@@ -13451,7 +13455,7 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="8" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="F127" s="8"/>
       <c r="G127" s="23" t="str">
@@ -13473,7 +13477,7 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="8" t="s">
-        <v>463</v>
+        <v>443</v>
       </c>
       <c r="F128" s="8"/>
       <c r="G128" s="23" t="str">
@@ -13498,7 +13502,7 @@
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="8" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="F129" s="8"/>
       <c r="G129" s="23" t="str">
@@ -13524,7 +13528,7 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="F130" s="8"/>
       <c r="G130" s="23" t="str">
@@ -13548,7 +13552,7 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="F131" s="8"/>
       <c r="G131" s="23" t="str">
@@ -13569,7 +13573,7 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="23" t="str">
@@ -13591,7 +13595,7 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="8" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="23" t="str">
@@ -13616,7 +13620,7 @@
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="F134" s="8"/>
       <c r="G134" s="23" t="str">
@@ -13643,7 +13647,7 @@
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="23" t="str">
@@ -13722,7 +13726,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -13734,7 +13738,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix: Chapter 3 Writting
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2026\C++\Signal_Lost\Signal_Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A96931F-5326-432E-9EC3-88DA61029DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEED3834-5C51-496A-AFF2-EA5226E1397E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters_Header" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="609">
   <si>
     <t>Chapter Name</t>
   </si>
@@ -1548,14 +1548,6 @@
 I guess it is.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Nothing that strikes my mi-[Wait=500] Oh wait![Wait=500][Space=2]_
-There are flyers lying here and there.[Wait=500] Let me try to catch one.[Wait=500][Space=2]
-...[Color=Gray]*Footsteps*[Color=White][Wait=500] ...Oof![Wait=500][Space=2]
-...[Wait=500]I got one! *Paper noises*...[Wait=500][Space=2]
-...Uhmm[Wait=500]...[Wait=500] It looks like a presentation of the animals of the zoo.[Wait=500][Space=2]
-It's weird but there are words written using markers on the snake's page.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>There's the first word [Color=Green]"BRSBNE"[Color=White].[Wait=500][Space=2]
 Then there's an arrow leading to the word [Color=Green]"DRWN"[Color=White].[Wait=500][Space=2]
 And the word [Color=Green]"PRTH"[Color=White] at the very end.[Wait=500][Space=2]
@@ -1665,21 +1657,9 @@
 Ouch?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I...[Wait=500] I just got stung by somthing behind my neck...[Wait=500][Space=2]
-What is it...[Wait=500] Uh?[Wait=500] It says "Snake veno-...[Wait=500][Space=2]
-OH MY GOD, IT'S A POISONNED DART!![Wait=500][Space=2]
-Oh shit, shit shit shit![Wait=500] I'm going to DIE POISONNED!![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Y-You're right![Wait=500] These plastic bottles might have something to do with it and...[Wait=500][Space=2]
 Oh lord, it looks like vials with syringes of medication...[Wait=500] Don't tell me I have to inject one of these things...[Wait=500][Space=2]
 Shit...[Wait=500] I can feel my consciouscness flying away...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>"O...[Wait=500] One has a label with "mRNA-1273"...[Wait=500][Space=2]
-The...[Wait=500] other one is "ASVS serum"...[Wait=500][Space=2]
-The last one has...[Wait=500] "Liquified HCN".[Wait=500][Space=2]
-Please hurry...[Wait=500] I don't want to die here...[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>I'm near the enclosure. It's really big![Wait=500] Looks like it's trying to remake a wild environment.[Wait=500][Space=2]
@@ -1721,12 +1701,6 @@
 I don't need this kind of joke now![Wait=500] I need you to take this situation seriously.[Wait=500][Space=2]
 Something is really after me and it's clear it's for no good...[Wait=500][Space=2]
 You're right on one thing...[Wait=500] I have to get out, AND FAST![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>What do you mean I'm "Imagining things"?[Wait=500][Space=2]_
-Do you think it was fake poison?[Wait=500] Fake pain?[Wait=500] Or maybe that this whole trap was set by the inca years ago?[Wait=500][Space=2]
-I'm not going to listen to your opinion anyway.[Wait=500] What I'm living is real...[Wait=500][Space=2]
-Why are you trying to convince me otherwise?...[Wait=500] Are you part of this?[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Why would this phone call the biggest ASSHOLE ON EARTH TO HELP ME![Wait=500][Space=2]
@@ -1876,12 +1850,6 @@
 ...[Wait=500] It seems that it comes from behind this one rusty door.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>...[Color=Gray]*Door handle noise*[Color=White]...[Wait=500][Space=2]
-...[Wait=500][Space=2]
-...[Wait=500] [Color=Gray]*Vomit noises*[Color=White]...[Wait=500][Space=2]
-OH MY-[Color=Gray]*Cough* *Cough*[Color=White]...[Wait=500] THERE ARE DEAD CORPSES ALL OVER THE GROUND![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I-...[Wait=500] I DON'T FREAKING KNOW![Wait=500][Space=2]_
 THEY ARE PILES OF DEAD BODIES AND YOU THINK THE FIRST QUESTIONS THAT COMES TO MY MIND IS![Wait=500][Space=2]
 "Oh! Why did they landed here? Did they die of pneumonia? How curious!"[Wait=500]...[Wait=500][Space=2]
@@ -2470,6 +2438,493 @@
 I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beginning, right?[Wait=500][Space=2]
 [Color=Gray]*SLAM*[Color=White]... OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
 [Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=2][Content=Okay, go when you're ready!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=3][TrustAdd=25][Content=No worries. I feel better knowing you're safe.]]
+[Choice2=[NextScene=5][TrustAdd=-25][Content=Your story still feels kinda weird to me...]]
+[Choice3=[NextScene=6][Content=It's true that I didn't expect to have this kind of call today!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=4][Content=Talking about that, this whole situation is trully unreal.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=7][TrustAdd=25][Content=Calm down, you'll be safe with me, I promise.]]
+[Choice2=[NextScene=9][TrustAdd=-25][Content=Keep quiet! Someone might hear you!]]
+[Choice3=[NextScene=11][TrustAdd=25][Content=All that matters is getting you out of here.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=4][Content=Don't worry, I believe your story, it just feels... unreal.]]
+[Choice2=[NextScene=10][TrustAdd=25][Content=I guess I'll be your talkable web browser from now on!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=4][Content=It's true, all of this is so unreal...]]
+[Choice2=[NextScene=8][TrustAdd=25][Content=I can assure you I'm real, if that's a relief for you.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=Nice! So, you're near the zoo now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=So, you're near the zoo now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=12][TrustAdd=-25][Content=Yes, try not to break your only connection to the outside world next time.]]
+[Choice2=[NextScene=13][TrustAdd=25][Content=It's okay. Try to keep your mind straight, now's not the time to act recklessly.]]
+[Choice3=[NextScene=14][TrustAdd=-25][Content=I'm trying to help you and this is what I get? I'll hang up if you continue like that.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=Let's explore the zoo since you're near it now, right?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=The zoo could give you the keys for getting out of here. You're approaching it right?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=It's pretty solid for sure. But how about the zoo?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=That's okay. You arrived now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=That's better. Now tell me, you're at the zoo?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=16][Content=Is there something else around?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=17][Content=What do they say?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=19][Content=Why are you pretending it's not you saying those things?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=17][Content=Right... So, what were those words again?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=24][Content=Go North.]]
+[Choice2=[NextScene=22][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=24][Content=Go West.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=22][Content=Go North.]]
+[Choice2=[NextScene=24][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=24][Content=Go West.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=24][Content=Go North.]]
+[Choice2=[NextScene=24][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=25][Content=Go West.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=17][Content=I made a mistake. Could you give me those words that were on the flyer?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=What do you see around you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=27][Content=The exit door could be your way out!]]
+[Choice2=[NextScene=28][Content=Is there something interesting with these palm trees?]]
+[Choice3=[NextScene=29][Content=Search for clues inside the reception desk.]]
+[Choice4=[NextScene=32][Content=Let's look at this glass enclosure.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=What can you see again?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=Let's ignore this for now. Is there something else around you?]]
+[Choice2=[NextScene=30][TrustAdd=-25][Content=Come on, keep reading!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=Leave somewhere else before you asphyxiate yourself.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=Okay, let's look what else is here.]]
+[Choice2=[NextScene=31][TrustAdd=-25][Content=You're kidding me? This must mean something!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=32][Content=Okay... Is there something else here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=34][Content=Now that you're educated, you can go inside!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=35][Content=What was that sound?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=36][Content=What was that?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=37][Content=Keep calm. It must be another puzzle!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=38][Content=Quick, tell me what are these bottles!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=40][Content=Y-You're not going to!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=42][Content=What was that? Who shot that dart in the first place?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=43][TrustAdd=-25][Content=GET OUT, HE'S OBSERVING YOU!]]
+[Choice2=[NextScene=44][TrustAdd=-25][Content=You're imagining things.]]
+[Choice3=[NextScene=47][TrustAdd=25][Content=You must be right.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=49][Content=Wasn't there an exit door?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=45][TrustAdd=-25][Content=Here you go, imagining things again.]]
+[Choice2=[NextScene=46][TrustAdd=-25][Content=No! What would I benefit from this anyway?]]
+[Choice3=[NextScene=48][Content=Yes, I am.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=49][Content=The biggest asshole on earth tells you to go check the exit door.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=49][Content=How about that exit door from before?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=50][Content=Let's enter!]]
+[Choice2=[NextScene=50][Content=That's freaking me out... Let's go back.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=51][Content=Hey? What happened? HEY?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=52][Content=Can't you go back to the vivarium?]]
+[Choice2=[NextScene=55][Content=I see... Where did you landed?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=53][Content=A monster you say?]]
+[Choice2=[NextScene=55][Content=Where are you now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=54][Content=What did it look like?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=54][Content=We'll get you out of here by moving forward.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=56][Content=You're under the island! Maybe you can access other parts of the city from here.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=57][Content=Huh? What did you say?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=58][Content=I-Is there a code near you by any chance?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=59][Content=Okay noted, now you'll have to listen to my instructions.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=60][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=61][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=62][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=63][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=65][Content=Go Left.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[Default=True][NextScene=66][Content=GO FRONT!]]
+[Choice2=[NextScene=66][Content=GO RIGHT!]]
+[Choice3=[NextScene=103][Content=GO LEFT!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=67][Content=Hey! Tell me you're still alive please!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=68][Content=What's around you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=69][Content=Can you get up and explore the place?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=70][Content=You guessed it.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=71][Content=Are you sure you have to open this one?...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=72][TrustAdd=-25][Content=Why are they here?]]
+[Choice2=[NextScene=72][TrustAdd=-25][Content=How did they die?]]
+[Choice3=[NextScene=73][Content=Who are they?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=73][Content=Are they this terrifying?]]
+[Choice2=[NextScene=74][TrustAdd=25][Content=Calm down! You're safe with me.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=76][NextSceneNoTrust=84][TrustNeed=75][Content=I don't understand that...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=75][Content=What do you mean by looking all the same?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=84][NextSceneNoTrust=76][TrustNeed=75][Content=Can it be that...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=77][Content=Don't lose hope, there must be a way to get you out of here.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=78][Content=You're speaking nonsense!]]
+[Choice2=[NextScene=79][Content=Are you... accusing me?]]
+[Choice3=[NextScene=79][Content=That's it, you're turning mad.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=79][Content=Are you okay?]]
+[Choice2=[NextScene=79][Content=What was that?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=80][Content=Climb back to the vent!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=81][TrustAdd=-25][Content=I can't do anything!]]
+[Choice2=[NextScene=81][TrustAdd=-25][Content=You're the one who jumped in the lion's den!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=83][TrustAdd=-25][Content=Oh no...]]
+[Choice2=[NextScene=83][TrustAdd=-25][Content=That's what you deserved.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=85][Content=My voice? What about it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=82][TrustAdd=-25][Content=GET OUT OF HERE!]]
+[Choice2=[NextScene=82][TrustAdd=-25][Content=I DIDN'T DO ANYTHING, I SWEAR!]]
+[Choice3=[NextScene=82][TrustAdd=-25][Content=That's for not believing me!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=86][Content=What's your theory?]]
+[Choice2=[NextScene=86][TrustAdd=-25][Content=Have you become insane?]]
+[Choice3=[NextScene=86][TrustAdd=25][Content=You might be right about that...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=87][Content=Is there anything more clues here?]]
+[Choice2=[NextScene=90][Content=I don't care about who you are, LET'S GET OUT!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=88][Content=Nutrient grinder?]]
+[Choice2=[NextScene=89][Content=Does that mean they might be other like us in here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=89][Content=So all of these dead bodies are... me?]]
+[Choice2=[NextScene=89][Content=But what about the monster from before. Was it a clone?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=90][Content=Is there a way to go back at the surface?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=91][Content=What's up? Why did you stop talking?]]
+[Choice1=[NextScene=91][Content=Hello? You're there?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=92][Content=Don't move.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=41][Content=Take the "ASVS Serum".]]
+[Choice2=[Default=True][NextScene=39][Content=Take the "Liquified HCN".]]
+[Choice3=[NextScene=39][Content=Take the "mRNA-1273".]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=93][Content=GO EAST!]]
+[Choice3=[NextScene=100][Content=GO SOUTH!]]
+[Choice4=[NextScene=100][Content=GO WEST!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=100][Content=GO EAST!]]
+[Choice3=[NextScene=94][Content=GO SOUTH!]]
+[Choice4=[NextScene=100][Content=GO WEST!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=100][Content=GO EAST!]]
+[Choice3=[NextScene=100][Content=GO SOUTH!]]
+[Choice4=[NextScene=95][Content=GO WEST!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=96][Content=HURRY!]]
+[Choice2=[NextScene=96][Content=DID IT WORKED?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=97][Content=It opened?]]
+[Choice2=[NextScene=97][Content=IT OPENED!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=98][Content=Wait, the signal's getting weaker!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=99][Content=I hope you'll be safe. Goodbye.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=101][Content=W-What is he talking about?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=102][Content=...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=104][Content=Where are you now?]]
+[Choice2=[NextScene=105][TrustAdd=25][Content=Are you safe?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=106][Content=Disfigured human?]]
+[Choice2=[NextScene=107][TrustAdd=25][Content=Right, take your time to breath.]]
+[Choice3=[NextScene=108][TrustAdd=-25][Content=I didn't know you were a soft belly.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=109][TrustAdd=-25][Content=Why did it chase you in the first place?]]
+[Choice2=[NextScene=110][Content=It might be better to get out of here since it might get out of the rubble.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=111][Content=Can you describe what's around you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=115][Content=You can't believe what?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=116][Content=Not so fast, it might be a trap!]]
+[Choice1=[NextScene=117][Content=What kind of boat is it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=118][Content=Focus now! Is there nothing else in this room?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=118][NextSceneNoTrust=130][TrustNeed=50][Content=Focus now! Is there nothing else in this room?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=119][Content=Try to-...]]
+[Choice2=[NextScene=119][Content=Go in-...]]
+[Choice3=[NextScene=119][Content=Hide from-...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=120][Content=Original? What does he mean?]]
+[Choice2=[NextScene=120][Content=What do you mean by creator?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=121][Content=I...]]
+[Choice2=[NextScene=121][Content=But...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=122][Content=HE'S GOING TO KILL YOU!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=123][TrustAdd=25][Content=FIGHT HIM!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=124][TrustAdd=25][Content=GIVE HIM WHAT HE DESERVES!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=125][Content=You killed him?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=126][Content=What are you going to do now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=127][Content=I hope you'll have a good trip on the sea!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=128][Content=Well then, I guess it's a goodbye.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=129][Content=See you around.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=131][Content=You want me to search on the internet?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=132][Content=Who is talking?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=133][Content=FIGHT BACK, DO SOMETHING!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=134][Content=No... It can't be...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=113][Content=It might be another trap then, can't you go back?]]
+[Choice2=[NextScene=114][Content=It's time to face another test it seems.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=26][Content=Seems dangerous... Let's see if there's more thing around before.]]
+[Choice2=[NextScene=33][Content=Is there more precisions on the sign?]]
+[Choice3=[NextScene=34][Content=Go see what's inside.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=17][Content=Okay... What were those words again?]]
+[Choice2=[NextScene=20][TrustAdd=-25][Content=Something weird is definitly going on...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=18][Content=What do you mean Australia?]]
+[Choice2=[NextScene=21][Content=Let's why this page deserves to be writing on in this snake's vivarium!]]</t>
+  </si>
+  <si>
+    <t>Nothing that strikes my mi-[Wait=500] Oh wait![Wait=500][Space=2]_
+There are flyers lying here and there.[Wait=500] Let me try to catch one.[Wait=500][Space=2]
+...[Color=Gray]*Footsteps*[Color=White][Wait=500] ...Oof![Wait=500][Space=2]
+...[Wait=500]I got one! [Color=Gray]*Paper noises*[Color=White]...[Wait=500][Space=2]
+...Uhmm[Wait=500]...[Wait=500] It looks like a presentation of the animals of the zoo.[Wait=500][Space=2]
+It's weird but there are words written using markers on the snake's page.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I...[Wait=500] I just got stung by somthing behind my neck...[Wait=500][Space=2]
+What is it...[Wait=500] Uh?[Wait=500] It says "Snake veno-"...[Wait=500][Space=2]
+OH MY GOD, IT'S A POISONNED DART!![Wait=500][Space=2]
+Oh shit, shit shit shit![Wait=500] I'm going to DIE POISONNED!![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>O...[Wait=500] One has a label with "mRNA-1273"...[Wait=500][Space=2]
+The...[Wait=500] other one is "ASVS serum"...[Wait=500][Space=2]
+The last one has...[Wait=500] "Liquified HCN".[Wait=500][Space=2]
+Please hurry...[Wait=500] I don't want to die here...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>What do you mean I'm "imagining things"?[Wait=500][Space=2]_
+Do you think it was fake poison?[Wait=500] Fake pain?[Wait=500] Or maybe that this whole trap was set by the inca years ago?[Wait=500][Space=2]
+I'm not going to listen to your opinion anyway.[Wait=500] What I'm living is real...[Wait=500][Space=2]
+Why are you trying to convince me otherwise?...[Wait=500] Are you part of this?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Color=Gray]*Door handle noise*[Color=White]...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+...[Wait=500] [Color=Gray]*Vomit noises*[Color=White]...[Wait=500][Space=2]
+OH MY-[Color=Gray]*Cough*[Color=White]... [Color=Gray]*Cough*[Color=White]...[Wait=500] THERE ARE DEAD CORPSES ALL OVER THE GROUND![Wait=500][Space=2]</t>
   </si>
 </sst>
 </file>
@@ -5103,8 +5558,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="B72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView topLeftCell="F67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5184,7 +5639,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
@@ -5591,7 +6046,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>34</v>
@@ -5767,7 +6222,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>50</v>
@@ -5951,7 +6406,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>51</v>
@@ -6191,7 +6646,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>59</v>
@@ -6341,7 +6796,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>63</v>
@@ -6428,7 +6883,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>42</v>
@@ -6485,7 +6940,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>65</v>
@@ -6513,7 +6968,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>66</v>
@@ -6541,7 +6996,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>67</v>
@@ -6570,7 +7025,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>68</v>
@@ -6627,7 +7082,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>69</v>
@@ -6697,7 +7152,7 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>45</v>
@@ -6987,7 +7442,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>75</v>
@@ -7042,7 +7497,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>77</v>
@@ -7247,7 +7702,7 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>84</v>
@@ -7333,8 +7788,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="E106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7574,7 +8029,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>291</v>
@@ -7602,7 +8057,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>159</v>
@@ -7741,7 +8196,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>294</v>
@@ -7994,7 +8449,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>300</v>
@@ -8048,7 +8503,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>300</v>
@@ -8214,7 +8669,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>305</v>
@@ -8298,7 +8753,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>164</v>
@@ -8413,7 +8868,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>168</v>
@@ -8662,7 +9117,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>173</v>
@@ -8728,7 +9183,7 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>175</v>
@@ -8760,7 +9215,7 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>176</v>
@@ -8824,7 +9279,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>179</v>
@@ -9155,7 +9610,7 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>186</v>
@@ -9184,7 +9639,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>310</v>
@@ -9212,7 +9667,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>187</v>
@@ -9410,7 +9865,7 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="8" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>194</v>
@@ -9494,7 +9949,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>196</v>
@@ -9574,7 +10029,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>198</v>
@@ -9916,7 +10371,7 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>311</v>
@@ -9985,7 +10440,7 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>210</v>
@@ -10407,7 +10862,7 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F108" s="13" t="s">
         <v>177</v>
@@ -10472,8 +10927,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="E72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10521,7 +10976,9 @@
       <c r="E2" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>482</v>
+      </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=1
@@ -10530,6 +10987,9 @@
 I guess I can go to the zoo, yeah.[Wait=500][Space=2]
 I don't see how going in any of these locations could help me escape this island.[Wait=500][Space=2]
 So whatever you'll choose might be the best.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=2][Content=Okay, go when you're ready!]]
 ]
 ]</v>
       </c>
@@ -10544,7 +11004,9 @@
       <c r="E3" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>483</v>
+      </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=2
@@ -10553,6 +11015,11 @@
 ...[Wait=500][Space=2]
 ...[Wait=500] Uhm...[Wait=500] Yeah...[Wait=500] I'm kinda sorry for the position I put you in with this call and everything.[Wait=500][Space=2]
 But it seems-[Wait=500] ...I didn't have that many choices.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=3][TrustAdd=25][Content=No worries. I feel better knowing you're safe.]]
+[Choice2=[NextScene=5][TrustAdd=-25][Content=Your story still feels kinda weird to me...]]
+[Choice3=[NextScene=6][Content=It's true that I didn't expect to have this kind of call today!]]
 ]
 ]</v>
       </c>
@@ -10567,13 +11034,18 @@
       <c r="E4" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>484</v>
+      </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=3
 [Content=
 T-Thanks...[Wait=500][Space=2]
 It's good to know I can rely on you,[Wait=500] especially in the kind of situation I'm in. So th-[Wait=500] Thanks, I guess...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=4][Content=Talking about that, this whole situation is trully unreal.]]
 ]
 ]</v>
       </c>
@@ -10588,7 +11060,9 @@
       <c r="E5" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>485</v>
+      </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=4
@@ -10599,6 +11073,11 @@
 Where the fuck am I?...[Wait=500] WHY IS NO ONE HERE TO ANSWER MY DAMN QUESTIONS?![Wait=500][Space=2]
 [Color=Gray]*Echoes fade in the distance*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=7][TrustAdd=25][Content=Calm down, you'll be safe with me, I promise.]]
+[Choice2=[NextScene=9][TrustAdd=-25][Content=Keep quiet! Someone might hear you!]]
+[Choice3=[NextScene=11][TrustAdd=25][Content=All that matters is getting you out of here.]]
+]
 ]</v>
       </c>
     </row>
@@ -10612,7 +11091,9 @@
       <c r="E6" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>486</v>
+      </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=5
@@ -10621,6 +11102,10 @@
 UGH![Wait=500] You know what?[Wait=500] It doesn't matter if you're not believing any of this.[Wait=500][Space=2]
 I just want you to stay with me since this place is filled with puzzles I could not solve alone.[Wait=500][Space=2]
 Sounds okay with you?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=4][Content=Don't worry, I believe your story, it just feels... unreal.]]
+[Choice2=[NextScene=10][TrustAdd=25][Content=I guess I'll be your talkable web browser from now on!]]
 ]
 ]</v>
       </c>
@@ -10635,7 +11120,9 @@
       <c r="E7" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>487</v>
+      </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=6
@@ -10646,6 +11133,10 @@
 ...[Wait=500][Space=2]
 I can't even tell if I'm dreaming or not.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=4][Content=It's true, all of this is so unreal...]]
+[Choice2=[NextScene=8][TrustAdd=25][Content=I can assure you I'm real, if that's a relief for you.]]
+]
 ]</v>
       </c>
     </row>
@@ -10659,7 +11150,9 @@
       <c r="E8" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>488</v>
+      </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=7
@@ -10671,6 +11164,9 @@
 [Color=Gray]*Breath*[Color=White]...[Wait=500][Space=2]
 Alright![Wait=500] I'm up to go![Wait=500] I think I can keep going thanks to you.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=15][Content=Nice! So, you're near the zoo now?]]
+]
 ]</v>
       </c>
     </row>
@@ -10684,7 +11180,9 @@
       <c r="E9" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>489</v>
+      </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=8
@@ -10695,6 +11193,9 @@
 I'll eventually work out why all of this is happening in the first place.[Wait=500][Space=2]
 But for now, let's just move forward.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=15][Content=So, you're near the zoo now?]]
+]
 ]</v>
       </c>
     </row>
@@ -10708,7 +11209,9 @@
       <c r="E10" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>490</v>
+      </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=9
@@ -10720,6 +11223,11 @@
 ...[Wait=500]Oh no, no, no, no, what have I done...[Wait=500] Please tell me you're still working...[Wait=500][Space=2]
 ...H-[Wait=500]Hello...[Wait=500] You still hear me?...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=12][TrustAdd=-25][Content=Yes, try not to break your only connection to the outside world next time.]]
+[Choice2=[NextScene=13][TrustAdd=25][Content=It's okay. Try to keep your mind straight, now's not the time to act recklessly.]]
+[Choice3=[NextScene=14][TrustAdd=-25][Content=I'm trying to help you and this is what I get? I'll hang up if you continue like that.]]
+]
 ]</v>
       </c>
     </row>
@@ -10733,7 +11241,9 @@
       <c r="E11" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>491</v>
+      </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=10
@@ -10741,6 +11251,9 @@
 Good one, clown.[Wait=500][Space=2]
 Anyway, I'm getting near the entrance of the zoo.[Wait=500][Space=2]
 It might be better if we focus on getting out of here more than joking around.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=15][Content=Let's explore the zoo since you're near it now, right?]]
 ]
 ]</v>
       </c>
@@ -10755,7 +11268,9 @@
       <c r="E12" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>492</v>
+      </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=11
@@ -10764,6 +11279,9 @@
 ...[Wait=500]If that's even possible.[Wait=500] I mean...[Wait=500][Space=2]
 Opening this trapdoor might be the only way out of here, but why is it here in the first place?[Wait=500][Space=2]
 I guess I won't have any answer if I don't go and see by myself.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=15][Content=The zoo could give you the keys for getting out of here. You're approaching it right?]]
 ]
 ]</v>
       </c>
@@ -10778,7 +11296,9 @@
       <c r="E13" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>493</v>
+      </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=12
@@ -10786,6 +11306,9 @@
 I'm so, so, so sorry.[Wait=500] I didn't mean to yell like that...[Wait=500][Space=2]
 What is this thing made of?[Wait=500][Space=2]
 I don't know how much this piece of junk can endure but I don't want to find out.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=15][Content=It's pretty solid for sure. But how about the zoo?]]
 ]
 ]</v>
       </c>
@@ -10800,7 +11323,9 @@
       <c r="E14" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>494</v>
+      </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=13
@@ -10808,6 +11333,9 @@
 R-Right,[Wait=500] you're right.[Wait=500][Space=2]
 I'm lucky this flip phone can handle this much.[Wait=500][Space=2]
 I think I can keep going now.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=15][Content=That's okay. You arrived now?]]
 ]
 ]</v>
       </c>
@@ -10822,13 +11350,18 @@
       <c r="E15" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>495</v>
+      </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=14
 [Content=
 NO PLEASE, I DON'T KNOW IF I COULD EVEN MAKE IT OUT ALIVE WITHOUT YOU![Wait=500][Space=2]
 O-Okay,[Wait=500] I'll be more careful from now on...[Wait=500] Please don't go.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=15][Content=That's better. Now tell me, you're at the zoo?]]
 ]
 ]</v>
       </c>
@@ -10843,7 +11376,9 @@
       <c r="E16" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>496</v>
+      </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=15
@@ -10855,6 +11390,9 @@
 ...[Wait=500]Is my brain fucked up for laughing at this?[Wait=500][Space=2]
 I guess it is.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=16][Content=Is there something else around?]]
+]
 ]</v>
       </c>
     </row>
@@ -10866,9 +11404,11 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="F17" s="8"/>
+        <v>604</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>497</v>
+      </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=16
@@ -10876,9 +11416,12 @@
 Nothing that strikes my mi-[Wait=500] Oh wait![Wait=500][Space=2]_
 There are flyers lying here and there.[Wait=500] Let me try to catch one.[Wait=500][Space=2]
 ...[Color=Gray]*Footsteps*[Color=White][Wait=500] ...Oof![Wait=500][Space=2]
-...[Wait=500]I got one! *Paper noises*...[Wait=500][Space=2]
+...[Wait=500]I got one! [Color=Gray]*Paper noises*[Color=White]...[Wait=500][Space=2]
 ...Uhmm[Wait=500]...[Wait=500] It looks like a presentation of the animals of the zoo.[Wait=500][Space=2]
 It's weird but there are words written using markers on the snake's page.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=17][Content=What do they say?]]
 ]
 ]</v>
       </c>
@@ -10891,9 +11434,11 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="F18" s="8"/>
+        <v>331</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>603</v>
+      </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=17
@@ -10904,6 +11449,10 @@
 Too bad I can't speak moon runes.[Wait=500][Space=2]
 [Color=Magenta][Beep=True]AuS[Wait=500][Beep=True]tRaLiA mI[Wait=500][Beep=True]gHt hAv[Wait=500][Beep=True]e sOmE[Wait=500][Beep=True]tHiNg tO[Wait=500][Beep=True]  dO wItH[Wait=500][Beep=True]  tHiS.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=18][Content=What do you mean Australia?]]
+[Choice2=[NextScene=21][Content=Let's why this page deserves to be writing on in this snake's vivarium!]]
+]
 ]</v>
       </c>
     </row>
@@ -10915,15 +11464,20 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" s="8"/>
+        <v>332</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>498</v>
+      </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=18
 [Content=
 Huh?[Wait=500] I said nothing about [Color=Green]Australia[Color=White].[Wait=500][Space=2]
 [Color=Magenta][Beep=True]ThO[Wait=500][Beep=True]se wOr[Wait=500][Beep=True]ds cOu[Wait=500][Beep=True]Ld bE[Wait=500][Beep=True]  rElAt[Wait=500][Beep=True]eD tO[Wait=500][Beep=True]  aUsTa[Wait=500][Beep=True]LiA mA[Wait=500][Beep=True]p, dO[Wait=500][Beep=True]n'T yOu[Wait=500][Beep=True]  tHiNk?[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=19][Content=Why are you pretending it's not you saying those things?]]
 ]
 ]</v>
       </c>
@@ -10936,9 +11490,11 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="F20" s="8"/>
+        <v>333</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>602</v>
+      </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=19
@@ -10948,6 +11504,10 @@
 Getting me OUT OF HERE![Wait=500][Space=2]
 [Color=Magenta][Beep=True]I'[Wait=500][Beep=True]Ll bE hE[Wait=500][Beep=True]re tO[Wait=500][Beep=True]  hElP yOu[Wait=500][Beep=True],  tHe oT[Wait=500][Beep=True]hEr oNe[Wait=500][Beep=True]  iS fO[Wait=500][Beep=True]lLoWiNg[Wait=500][Beep=True]  yOu.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=17][Content=Okay... What were those words again?]]
+[Choice2=[NextScene=20][TrustAdd=-25][Content=Something weird is definitly going on...]]
+]
 ]</v>
       </c>
     </row>
@@ -10959,15 +11519,20 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="F21" s="8"/>
+        <v>334</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>499</v>
+      </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=20
 [Content=
 No shit Sherlock![Wait=500] Everything's weird in here.[Wait=500][Space=2]
 I need your help now, so prove me you're not crazy and you can be helpful![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=17][Content=Right... So, what were those words again?]]
 ]
 ]</v>
       </c>
@@ -10980,9 +11545,11 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F22" s="8"/>
+        <v>335</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>500</v>
+      </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=21
@@ -10990,6 +11557,12 @@
 Seeing what's inside this vivarium might be the best lead we have, you're right.[Wait=500][Space=2]
 Even if these words marked very clearly on this flyers are extremly suspiscious, I guess we have no choice.[Wait=500][Space=2]
 So? Where should I be heading now?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=24][Content=Go North.]]
+[Choice2=[NextScene=22][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=24][Content=Go West.]]
 ]
 ]</v>
       </c>
@@ -11002,9 +11575,11 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="F23" s="8"/>
+        <v>336</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>501</v>
+      </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=22
@@ -11014,6 +11589,12 @@
 Like, I feel that I'm the one being observed like an animal even if I'm the one outside of these cages.[Wait=500][Space=2]
 Enough weird and paranoïd thoughts.[Wait=500] What then?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=22][Content=Go North.]]
+[Choice2=[NextScene=24][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=24][Content=Go West.]]
+]
 ]</v>
       </c>
     </row>
@@ -11025,9 +11606,11 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="F24" s="8"/>
+        <v>337</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>502</v>
+      </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=23
@@ -11038,6 +11621,12 @@
 Too bad it's day time...[Wait=500] And that I haven't got a fucking idea how star triangulation works in the first place.[Wait=500][Space=2]
 Anyway, where should I go next?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=24][Content=Go North.]]
+[Choice2=[NextScene=24][Content=Go East.]]
+[Choice3=[NextScene=24][Content=Go South.]]
+[Choice4=[NextScene=25][Content=Go West.]]
+]
 ]</v>
       </c>
     </row>
@@ -11049,9 +11638,11 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="F25" s="8"/>
+        <v>338</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>503</v>
+      </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=24
@@ -11062,6 +11653,9 @@
 ...[Wait=500][Space=2]
 ...Well shit.[Wait=500] I'm somehow back at the entrance.[Wait=500] Nice direction you gave me there...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=17][Content=I made a mistake. Could you give me those words that were on the flyer?]]
+]
 ]</v>
       </c>
     </row>
@@ -11073,9 +11667,11 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="F26" s="8"/>
+        <v>339</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>504</v>
+      </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=25
@@ -11087,6 +11683,9 @@
 Well, that's anti-climatic![Wait=500] I expected to be bit by a viper or something.[Wait=500][Space=2]
 [Color=Magenta][Beep=True]I hO[Wait=500][Beep=True]pE yOu'[Wait=500][Beep=True]ll rEm[Wait=500][Beep=True]eMbEr  tHe[Wait=500][Beep=True]  wAy bA[Wait=500][Beep=True]cK.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=26][Content=What do you see around you?]]
+]
 ]</v>
       </c>
     </row>
@@ -11098,9 +11697,11 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="F27" s="8"/>
+        <v>340</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>505</v>
+      </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=26
@@ -11110,6 +11711,12 @@
 There are severals palm trees here and there and a reception desk over here.[Wait=500][Space=2]
 What should I do?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=27][Content=The exit door could be your way out!]]
+[Choice2=[NextScene=28][Content=Is there something interesting with these palm trees?]]
+[Choice3=[NextScene=29][Content=Search for clues inside the reception desk.]]
+[Choice4=[NextScene=32][Content=Let's look at this glass enclosure.]]
+]
 ]</v>
       </c>
     </row>
@@ -11121,9 +11728,11 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="F28" s="8"/>
+        <v>341</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>506</v>
+      </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=27
@@ -11133,6 +11742,9 @@
 What kind of shit-brained buffoon puts a freaking renforced chain on an emergency exit?[Wait=500][Space=2]
 ...[Wait=500]Hope there is something to break it down near there.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=26][Content=What can you see again?]]
+]
 ]</v>
       </c>
     </row>
@@ -11144,9 +11756,11 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="F29" s="8"/>
+        <v>342</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>507</v>
+      </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=28
@@ -11156,6 +11770,10 @@
 "GET ME OUT, HE'S OBSERVING ME, I CAN FEEL HIM PLAYING WITH MY MIND"...[Wait=500][Space=2]
 ...[Wait=500]Nope, nope nope nope,[Wait=500] that's it.[Wait=500] I don't want to read more of it.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=26][Content=Let's ignore this for now. Is there something else around you?]]
+[Choice2=[NextScene=30][TrustAdd=-25][Content=Come on, keep reading!]]
+]
 ]</v>
       </c>
     </row>
@@ -11167,9 +11785,11 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="F30" s="8"/>
+        <v>343</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>508</v>
+      </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=29
@@ -11180,6 +11800,9 @@
 I didn't even move these papers that much,[Wait=500] why is there so much dust flying around?[Wait=500][Space=2]
 [Color=Gray]*Cough*[Color=White]...[Wait=500] It's wei-[Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=26][Content=Leave somewhere else before you asphyxiate yourself.]]
+]
 ]</v>
       </c>
     </row>
@@ -11191,9 +11814,11 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="F31" s="8"/>
+        <v>344</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>509</v>
+      </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=30
@@ -11203,6 +11828,10 @@
 ...[Wait=500] Seriously...[Wait=500]I-I'm trembling in fear right now...[Wait=500][Space=2]
 L-Let's tell that this thing never existed.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=26][Content=Okay, let's look what else is here.]]
+[Choice2=[NextScene=31][TrustAdd=-25][Content=You're kidding me? This must mean something!]]
+]
 ]</v>
       </c>
     </row>
@@ -11214,9 +11843,11 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="F32" s="8"/>
+        <v>345</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>510</v>
+      </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=31
@@ -11226,6 +11857,9 @@
 I feel unsafe...[Wait=500][Space=2]
 And watched...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=32][Content=Okay... Is there something else here?]]
+]
 ]</v>
       </c>
     </row>
@@ -11237,9 +11871,11 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="F33" s="8"/>
+        <v>350</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>601</v>
+      </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=32
@@ -11247,6 +11883,11 @@
 I'm near the enclosure. It's really big![Wait=500] Looks like it's trying to remake a wild environment.[Wait=500][Space=2]
 There's a sign near the door with [Color=Green]"WATCH OUT, VENIMOUS TIGER-SNAKES INSIDE"[Color=White] marked on it.[Wait=500][Space=2]
 Normally I would freak out at this point but I know there's no living think anywhere here![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=26][Content=Seems dangerous... Let's see if there's more thing around before.]]
+[Choice2=[NextScene=33][Content=Is there more precisions on the sign?]]
+[Choice3=[NextScene=34][Content=Go see what's inside.]]
 ]
 ]</v>
       </c>
@@ -11259,9 +11900,11 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F34" s="8"/>
+        <v>346</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>511</v>
+      </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=33
@@ -11271,6 +11914,9 @@
 The snake’s venom, which contains a blood-clotting agent as well as a nerve paralyzer, is potentially fatal to humans.[Wait=500][Space=2]
 immediate injection of anti-venom is the only way to make it out without irreversible damage".[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=34][Content=Now that you're educated, you can go inside!]]
+]
 ]</v>
       </c>
     </row>
@@ -11282,9 +11928,11 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="F35" s="8"/>
+        <v>347</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>512</v>
+      </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=34
@@ -11292,6 +11940,9 @@
 It's weird to put a foot inside an animal enclosure.[Wait=500][Space=2]
 Feels like I'm the one being wa-[Color=Gray]*THUMB*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500] Oh no...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=35][Content=What was that sound?]]
 ]
 ]</v>
       </c>
@@ -11304,9 +11955,11 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="F36" s="8"/>
+        <v>348</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>513</v>
+      </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=35
@@ -11317,6 +11970,9 @@
 WHO DID THA-...[Wait=500][Space=2]
 Ouch?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=36][Content=What was that?]]
+]
 ]</v>
       </c>
     </row>
@@ -11328,17 +11984,22 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="F37" s="8"/>
+        <v>605</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>514</v>
+      </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=36
 [Content=
 I...[Wait=500] I just got stung by somthing behind my neck...[Wait=500][Space=2]
-What is it...[Wait=500] Uh?[Wait=500] It says "Snake veno-...[Wait=500][Space=2]
+What is it...[Wait=500] Uh?[Wait=500] It says "Snake veno-"...[Wait=500][Space=2]
 OH MY GOD, IT'S A POISONNED DART!![Wait=500][Space=2]
 Oh shit, shit shit shit![Wait=500] I'm going to DIE POISONNED!![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=37][Content=Keep calm. It must be another puzzle!]]
 ]
 ]</v>
       </c>
@@ -11351,9 +12012,11 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F38" s="8"/>
+        <v>349</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>515</v>
+      </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=37
@@ -11362,6 +12025,9 @@
 Oh lord, it looks like vials with syringes of medication...[Wait=500] Don't tell me I have to inject one of these things...[Wait=500][Space=2]
 Shit...[Wait=500] I can feel my consciouscness flying away...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=38][Content=Quick, tell me what are these bottles!]]
+]
 ]</v>
       </c>
     </row>
@@ -11377,19 +12043,26 @@
         <v>60</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="F39" s="8"/>
+        <v>606</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>566</v>
+      </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=38
 [Connection=2][Timer=60]
 [Content=
-"O...[Wait=500] One has a label with "mRNA-1273"...[Wait=500][Space=2]
+O...[Wait=500] One has a label with "mRNA-1273"...[Wait=500][Space=2]
 The...[Wait=500] other one is "ASVS serum"...[Wait=500][Space=2]
 The last one has...[Wait=500] "Liquified HCN".[Wait=500][Space=2]
 Please hurry...[Wait=500] I don't want to die here...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=41][Content=Take the "ASVS Serum".]]
+[Choice2=[Default=True][NextScene=39][Content=Take the "Liquified HCN".]]
+[Choice3=[NextScene=39][Content=Take the "mRNA-1273".]]
+]
 ]</v>
       </c>
     </row>
@@ -11403,9 +12076,11 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="F40" s="8"/>
+        <v>351</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>516</v>
+      </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=39
@@ -11418,6 +12093,9 @@
 I don't feel so good...[Wait=500][Space=2]
 ...[Wait=500] I don't want to...[Wait=500] die...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=40][Content=Y-You're not going to!]]
+]
 ]</v>
       </c>
     </row>
@@ -11431,9 +12109,11 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="F41" s="8"/>
+        <v>352</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=40
@@ -11447,6 +12127,12 @@
 [Color=Red]{YOU FAILED TO FIND THE RIGHT MEDICATION. MAYBE IF YOU'D TRIED HARDER?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -11460,9 +12146,11 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="F42" s="8"/>
+        <v>353</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>518</v>
+      </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=41
@@ -11475,6 +12163,9 @@
 I-[Wait=500] I think it worked![Wait=500] I don't feel pain anymore.[Wait=500][Space=2]
 ...[Wait=500] Looks like the door of the cage is open again too...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=42][Content=What was that? Who shot that dart in the first place?]]
+]
 ]</v>
       </c>
     </row>
@@ -11486,9 +12177,11 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="F43" s="8"/>
+        <v>354</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>519</v>
+      </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=42
@@ -11496,6 +12189,11 @@
 I...[Wait=500] I don't remember where it came from.[Wait=500][Space=2]
 But the fact that there was a serum to counter this venom in the first place is...[Wait=500][Space=2]
 Yeah, I'm not here by coincidence.[Wait=500] Someone's definitly trying to play with me.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=43][TrustAdd=-25][Content=GET OUT, HE'S OBSERVING YOU!]]
+[Choice2=[NextScene=44][TrustAdd=-25][Content=You're imagining things.]]
+[Choice3=[NextScene=47][TrustAdd=25][Content=You must be right.]]
 ]
 ]</v>
       </c>
@@ -11508,9 +12206,11 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F44" s="8"/>
+        <v>355</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>520</v>
+      </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=43
@@ -11520,6 +12220,9 @@
 Something is really after me and it's clear it's for no good...[Wait=500][Space=2]
 You're right on one thing...[Wait=500] I have to get out, AND FAST![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=49][Content=Wasn't there an exit door?]]
+]
 ]</v>
       </c>
     </row>
@@ -11531,17 +12234,24 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="F45" s="8"/>
+        <v>607</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>521</v>
+      </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=44
 [Content=
-What do you mean I'm "Imagining things"?[Wait=500][Space=2]_
+What do you mean I'm "imagining things"?[Wait=500][Space=2]_
 Do you think it was fake poison?[Wait=500] Fake pain?[Wait=500] Or maybe that this whole trap was set by the inca years ago?[Wait=500][Space=2]
 I'm not going to listen to your opinion anyway.[Wait=500] What I'm living is real...[Wait=500][Space=2]
 Why are you trying to convince me otherwise?...[Wait=500] Are you part of this?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=45][TrustAdd=-25][Content=Here you go, imagining things again.]]
+[Choice2=[NextScene=46][TrustAdd=-25][Content=No! What would I benefit from this anyway?]]
+[Choice3=[NextScene=48][Content=Yes, I am.]]
 ]
 ]</v>
       </c>
@@ -11554,9 +12264,11 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="F46" s="8"/>
+        <v>356</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>522</v>
+      </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=45
@@ -11564,6 +12276,9 @@
 Why would this phone call the biggest ASSHOLE ON EARTH TO HELP ME![Wait=500][Space=2]
 ...[Wait=500] I don't care anyway.[Wait=500] As long as you prevent me from dying like you did before I'm not going to complain...[Wait=500][Space=2]
 But it might be good if you start acting like you see me as a human being instead of a clown for once.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=49][Content=The biggest asshole on earth tells you to go check the exit door.]]
 ]
 ]</v>
       </c>
@@ -11576,9 +12291,11 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="F47" s="8"/>
+        <v>357</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>523</v>
+      </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=46
@@ -11589,6 +12306,9 @@
 Yeah, I guess I work with that for now.[Wait=500][Space=2]
 So?[Wait=500] It's time to get the fuck out of here before some bullshit puzzle happens again, right?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=49][Content=How about that exit door from before?]]
+]
 ]</v>
       </c>
     </row>
@@ -11600,15 +12320,20 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="F48" s="8"/>
+        <v>358</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>520</v>
+      </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=47
 [Content=
 If you're thinking the same as me, I think It's best if I follow my instinct and get out of here QUICK![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=49][Content=Wasn't there an exit door?]]
+]
 ]</v>
       </c>
     </row>
@@ -11622,9 +12347,11 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F49" s="8"/>
+        <v>359</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=48
@@ -11639,6 +12366,12 @@
 [Color=Red]{YOU HAVE LOST HIS TRUST. MAYBE THERE IS A BETTER CHOICE?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -11650,9 +12383,11 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="F50" s="8"/>
+        <v>360</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=49
@@ -11662,6 +12397,10 @@
 ...[Wait=500] The door...[Wait=500] It has been broke down...[Wait=500] Now it's wide open.[Wait=500][Space=2]
 I-It means someone kicked it down while I was inside the glass enclosure...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=50][Content=Let's enter!]]
+[Choice2=[NextScene=50][Content=That's freaking me out... Let's go back.]]
+]
 ]</v>
       </c>
     </row>
@@ -11673,15 +12412,20 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="F51" s="8"/>
+        <v>361</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>525</v>
+      </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=50
 [Content=
 I mean...[Wait=500] It might be better to go baAAAH WHAT THE FUCK!!!![Wait=500][Space=2]
 [Color=Gray]*Running sounds*[Color=White]...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=51][Content=Hey? What happened? HEY?!]]
 ]
 ]</v>
       </c>
@@ -11694,9 +12438,11 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="F52" s="8"/>
+        <v>362</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>526</v>
+      </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=51
@@ -11706,6 +12452,10 @@
 THERE WAS A SILHOUETTE LURKING BEHIND ME IN THE VIVARIUM![Wait=500][Space=2]
 I mechanicly ran through that damn door and got as far as possible.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=52][Content=Can't you go back to the vivarium?]]
+[Choice2=[NextScene=55][Content=I see... Where did you landed?]]
+]
 ]</v>
       </c>
     </row>
@@ -11717,9 +12467,11 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="F53" s="8"/>
+        <v>363</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>527</v>
+      </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=52
@@ -11730,6 +12482,10 @@
 Secondly, THERE WAS A FREACKING MONSTER OUT THERE AND I DON’T WANT TO MEET IT AGAIN![Wait=500][Space=2]
 Is that enough for you?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=53][Content=A monster you say?]]
+[Choice2=[NextScene=55][Content=Where are you now?]]
+]
 ]</v>
       </c>
     </row>
@@ -11741,9 +12497,11 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="F54" s="8"/>
+        <v>364</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>528</v>
+      </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=53
@@ -11751,6 +12509,9 @@
 Y-Yeah...[Wait=500] I can’t find another word to describe this thing.[Wait=500][Space=2]
 I’m sure that it was not my imagination...[Wait=500] I think...[Wait=500][Space=2]
 ...[Wait=500] Great, now you make me doubt of myself.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=54][Content=What did it look like?]]
 ]
 ]</v>
       </c>
@@ -11763,9 +12524,11 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="F55" s="8"/>
+        <v>365</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>529</v>
+      </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=54
@@ -11773,6 +12536,9 @@
 I only saw a silhoutte, but it was enough to activate my survival instinct.[Wait=500][Space=2]
 This thing had human forms but something was clearly off, I don’t know what.[Wait=500][Space=2]
 ...[Wait=500] Why can’t I wake up from this nightmare?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=54][Content=We'll get you out of here by moving forward.]]
 ]
 ]</v>
       </c>
@@ -11785,9 +12551,11 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F56" s="8"/>
+        <v>366</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>530</v>
+      </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=55
@@ -11795,6 +12563,9 @@
 Yes, uhm...[Wait=500] I landed in some sort of tunnels.[Wait=500][Space=2]
 It smells horrible, almost like the rotten food in the supermarket back then.[Wait=500][Space=2]
 There are several different path in here.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=56][Content=You're under the island! Maybe you can access other parts of the city from here.]]
 ]
 ]</v>
       </c>
@@ -11807,9 +12578,11 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="F57" s="8"/>
+        <v>367</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>531</v>
+      </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=56
@@ -11817,6 +12590,9 @@
 That’s a good idea, but where should I go?[Wait=500][Space=2]
 I have no idea where these paths will lead[Wait=500][Space=2]
 [Color=Magenta][Beep=True]Us[Wait=500][Beep=True]e tHe[Wait=500][Beep=True]  cO[Wait=500][Beep=True]dE.[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=57][Content=Huh? What did you say?]]
 ]
 ]</v>
       </c>
@@ -11829,9 +12605,11 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="F58" s="8"/>
+        <v>368</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>532</v>
+      </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=57
@@ -11839,6 +12617,9 @@
 ...[Wait=500] What?[Wait=500][Space=2]
 Why did you tell what?[Wait=500] I thought I was being clear.[Wait=500][Space=2]
 [Color=Magenta][Beep=True]Fi[Wait=500][Beep=True]nD tHe[Wait=500][Beep=True]  cO[Wait=500][Beep=True]dE.[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=58][Content=I-Is there a code near you by any chance?]]
 ]
 ]</v>
       </c>
@@ -11851,9 +12632,11 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="F59" s="8"/>
+        <v>369</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>533</v>
+      </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=58
@@ -11866,6 +12649,9 @@
 C = RIGHT"[Color=White]...[Wait=500][Space=2]
 [Color=Magenta][Beep=True]ReMe[Wait=500][Beep=True]mBeR iT[Wait=500][Beep=True],  iT wIlL[Wait=500][Beep=True]  nOt aPp[Wait=500][Beep=True]eAr aG[Wait=500][Beep=True]aIn.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=59][Content=Okay noted, now you'll have to listen to my instructions.]]
+]
 ]</v>
       </c>
     </row>
@@ -11877,9 +12663,11 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="F60" s="8"/>
+        <v>370</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>534</v>
+      </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=59
@@ -11887,6 +12675,11 @@
 B-But how did you know there was-...[Wait=500][Space=2]
 Fine...[Wait=500] Asking more questions will only confuse me more.[Wait=500][Space=2]
 So where should I go first?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=60][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]
 ]
 ]</v>
       </c>
@@ -11899,15 +12692,22 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="F61" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>535</v>
+      </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=60
 [Content=
 Okay, front it is.[Wait=500][Space=2]
 What then?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=61][Content=Go Left.]]
 ]
 ]</v>
       </c>
@@ -11920,9 +12720,11 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="F62" s="8"/>
+        <v>372</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>536</v>
+      </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=61
@@ -11932,6 +12734,11 @@
 Sorry, I thought a bit of humour would be nice, but I was wrong.[Wait=500][Space=2]
 What next?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=62][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]
+]
 ]</v>
       </c>
     </row>
@@ -11943,9 +12750,11 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="F63" s="8"/>
+        <v>373</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>537</v>
+      </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=62
@@ -11953,6 +12762,11 @@
 Front again.[Wait=500][Space=2]
 Oh Lord, why does it have to smell that much in here![Wait=500][Space=2]
 Hurry, where should I go?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=63][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]
 ]
 ]</v>
       </c>
@@ -11965,15 +12779,22 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="F64" s="8"/>
+        <v>374</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>538</v>
+      </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=63
 [Content=
 Alright, that's right, right?[Wait=500][Space=2]
 And how about right now?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=64][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=66][Content=Go Left.]]
 ]
 ]</v>
       </c>
@@ -11986,9 +12807,11 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="F65" s="8"/>
+        <v>375</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>539</v>
+      </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
         <v>[Scene=64
@@ -11996,6 +12819,11 @@
 Front is...[Wait=500] uh...[Wait=500] nah.[Wait=500] I don't have any puns on this one.[Wait=500][Space=2]
 Tell me what's next.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=66][Content=Go Front.]]
+[Choice2=[NextScene=66][Content=Go Right.]]
+[Choice3=[NextScene=65][Content=Go Left.]]
+]
 ]</v>
       </c>
     </row>
@@ -12011,9 +12839,11 @@
         <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F66" s="8"/>
+        <v>376</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>540</v>
+      </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G74" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=65
@@ -12025,6 +12855,11 @@
 Oh no...[Wait=500] OH DAMN DAMN DAMN DAMN IT'S RUNNING TOWARDS ME!!![Wait=500][Space=2]
 WHERE SHOULD I RUN QUICK!!![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[Default=True][NextScene=66][Content=GO FRONT!]]
+[Choice2=[NextScene=66][Content=GO RIGHT!]]
+[Choice3=[NextScene=103][Content=GO LEFT!]]
+]
 ]</v>
       </c>
     </row>
@@ -12038,9 +12873,11 @@
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="F67" s="8"/>
+        <v>377</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>541</v>
+      </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=66
@@ -12052,6 +12889,9 @@
 [Color=Gray]*COLLAPSING RUCKUS*[Color=White]...[Wait=500][Space=2]
 WOAAAAAAH SHIIIII-[Color=Gray]*THUMB*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=67][Content=Hey! Tell me you're still alive please!]]
+]
 ]</v>
       </c>
     </row>
@@ -12065,9 +12905,11 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="F68" s="8"/>
+        <v>378</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>542</v>
+      </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=67
@@ -12078,6 +12920,9 @@
 That hurts as hell...[Wait=500] I thing I broke a rib or something like that...[Wait=500][Space=2]
 Where did I landed?[Wait=500] OH MY GOD IT STINKS SO MUCH![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=68][Content=What's around you?]]
+]
 ]</v>
       </c>
     </row>
@@ -12091,9 +12936,11 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="F69" s="8"/>
+        <v>379</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>543</v>
+      </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=68
@@ -12103,6 +12950,9 @@
 I-I'm in-OUCH!-...[Wait=500] In a white room.[Wait=500] The lights work in here...[Wait=500] There's a door at the back.[Wait=500][Space=2]
 ...I feel like I'm not welcome here.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=69][Content=Can you get up and explore the place?]]
+]
 ]</v>
       </c>
     </row>
@@ -12114,9 +12964,11 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="F70" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>544</v>
+      </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=69
@@ -12124,6 +12976,9 @@
 I'll try...[Wait=500][Space=2]
 ...[Wait=500] OH! That hurts...[Wait=500] Okay... I'm standing up...[Wait=500][Space=2]
 I guess you'll ask me what's behind the door right?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=70][Content=You guessed it.]]
 ]
 ]</v>
       </c>
@@ -12136,9 +12991,11 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F71" s="8"/>
+        <v>381</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>545</v>
+      </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=70
@@ -12149,6 +13006,9 @@
 This horrible odor...[Wait=500] It smells more and more as I'm moving through the hallway...[Wait=500][Space=2]
 ...[Wait=500] It seems that it comes from behind this one rusty door.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=71][Content=Are you sure you have to open this one?...]]
+]
 ]</v>
       </c>
     </row>
@@ -12160,9 +13020,11 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="F72" s="8"/>
+        <v>608</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>546</v>
+      </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=71
@@ -12170,7 +13032,12 @@
 ...[Color=Gray]*Door handle noise*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ...[Wait=500] [Color=Gray]*Vomit noises*[Color=White]...[Wait=500][Space=2]
-OH MY-[Color=Gray]*Cough* *Cough*[Color=White]...[Wait=500] THERE ARE DEAD CORPSES ALL OVER THE GROUND![Wait=500][Space=2]
+OH MY-[Color=Gray]*Cough*[Color=White]... [Color=Gray]*Cough*[Color=White]...[Wait=500] THERE ARE DEAD CORPSES ALL OVER THE GROUND![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=72][TrustAdd=-25][Content=Why are they here?]]
+[Choice2=[NextScene=72][TrustAdd=-25][Content=How did they die?]]
+[Choice3=[NextScene=73][Content=Who are they?]]
 ]
 ]</v>
       </c>
@@ -12183,9 +13050,11 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="F73" s="8"/>
+        <v>382</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>547</v>
+      </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=72
@@ -12195,6 +13064,10 @@
 "Oh! Why did they landed here? Did they die of pneumonia? How curious!"[Wait=500]...[Wait=500][Space=2]
 NO, I'M SCARED, I WANT TO GET OUT OF HERE![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=73][Content=Are they this terrifying?]]
+[Choice2=[NextScene=74][TrustAdd=25][Content=Calm down! You're safe with me.]]
+]
 ]</v>
       </c>
     </row>
@@ -12206,9 +13079,11 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="F74" s="13"/>
+        <v>383</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>548</v>
+      </c>
       <c r="G74" s="24" t="str">
         <f t="shared" si="2"/>
         <v>[Scene=73
@@ -12218,6 +13093,9 @@
 ...[Wait=500] Why do they have the same clothes, the same body traits as...[Wait=500] me?[Wait=500] WHY DO THEY LOOK LIKE ME?![Wait=500][Space=2]
 It's just a nightmare oh my god.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=76][NextSceneNoTrust=84][TrustNeed=75][Content=I don't understand that...]]
+]
 ]</v>
       </c>
     </row>
@@ -12229,15 +13107,20 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F75" s="8"/>
+        <v>384</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>549</v>
+      </c>
       <c r="G75" s="23" t="str">
         <f>"[Scene=" &amp; A75 &amp; IF(OR(B75&lt;&gt;"",C75&lt;&gt;"",D75&lt;&gt;""),CHAR(10),"") &amp; IF(B75&lt;&gt;"","[BeepBack=" &amp; B75 &amp; "]","") &amp; IF(C75&lt;&gt;"","[Connection=" &amp; C75 &amp; "]","") &amp; IF(D75&lt;&gt;"","[Timer=" &amp; D75 &amp; "]","") &amp; IF(E75&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E75 &amp; CHAR(10) &amp; "]","") &amp; IF(F75&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F75 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=74
 [Content=
 I-I'm trying, but I'm terrified![Wait=500] There was some monster chasing me just before![Wait=500][Space=2]
 Now I'm inside this weird underground place filled with dead bodies looking all the same![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=75][Content=What do you mean by looking all the same?]]
 ]
 ]</v>
       </c>
@@ -12250,9 +13133,11 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="F76" s="8"/>
+        <v>385</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>550</v>
+      </c>
       <c r="G76" s="23" t="str">
         <f>"[Scene=" &amp; A76 &amp; IF(OR(B76&lt;&gt;"",C76&lt;&gt;"",D76&lt;&gt;""),CHAR(10),"") &amp; IF(B76&lt;&gt;"","[BeepBack=" &amp; B76 &amp; "]","") &amp; IF(C76&lt;&gt;"","[Connection=" &amp; C76 &amp; "]","") &amp; IF(D76&lt;&gt;"","[Timer=" &amp; D76 &amp; "]","") &amp; IF(E76&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E76 &amp; CHAR(10) &amp; "]","") &amp; IF(F76&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F76 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=75
@@ -12260,6 +13145,9 @@
 What do I mean?[Wait=500] I mean they all wear the same clothes, have the same facial features, have the same body trait...[Wait=500][Space=2]
 ...[Wait=500] Wait...[Wait=500] Why do they have the same clothes as...[Wait=500] me?[Wait=500][Space=2]
 No.[Wait=500] No, no, no it can't be, that's IMPOSSIBLE![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=84][NextSceneNoTrust=76][TrustNeed=75][Content=Can it be that...]]
 ]
 ]</v>
       </c>
@@ -12272,9 +13160,11 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="F77" s="8"/>
+        <v>386</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>551</v>
+      </c>
       <c r="G77" s="23" t="str">
         <f t="shared" ref="G77:G83" si="3">"[Scene=" &amp; A77 &amp; IF(OR(B77&lt;&gt;"",C77&lt;&gt;"",D77&lt;&gt;""),CHAR(10),"") &amp; IF(B77&lt;&gt;"","[BeepBack=" &amp; B77 &amp; "]","") &amp; IF(C77&lt;&gt;"","[Connection=" &amp; C77 &amp; "]","") &amp; IF(D77&lt;&gt;"","[Timer=" &amp; D77 &amp; "]","") &amp; IF(E77&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E77 &amp; CHAR(10) &amp; "]","") &amp; IF(F77&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F77 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=76
@@ -12284,6 +13174,9 @@
 They are clones, and so am I...[Wait=500][Space=2]
 We're just copies of you, played with in some kind of experiment.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=77][Content=Don't lose hope, there must be a way to get you out of here.]]
+]
 ]</v>
       </c>
     </row>
@@ -12295,9 +13188,11 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="F78" s="8"/>
+        <v>387</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>552</v>
+      </c>
       <c r="G78" s="23" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=77
@@ -12305,6 +13200,11 @@
 S-SHUT UP![Wait=500] YOU KNEW ALL ALONG![Wait=500] You're leading all of this right?[Wait=500][Space=2]
 You cloned yourself for some kind of experiment?[Wait=500] It's fun seeing yourself suffer right?[Wait=500][Space=2]
 I'm getting out of here, no matter what you say![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=78][Content=You're speaking nonsense!]]
+[Choice2=[NextScene=79][Content=Are you... accusing me?]]
+[Choice3=[NextScene=79][Content=That's it, you're turning mad.]]
 ]
 ]</v>
       </c>
@@ -12317,9 +13217,11 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="F79" s="8"/>
+        <v>388</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>553</v>
+      </c>
       <c r="G79" s="23" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=78
@@ -12329,6 +13231,10 @@
 [Color=Gray]*Metallic noises*[Color=White]...[Wait=500] You-humpf... You didn't expected me to go through the vents huh?[Wait=500][Space=2]
 Try to kill me now that you don't know [Color=Gray]*Crack*[Color=White] where I-[Color=Gray]*CRASH*[Color=White] AAAAAA-[Color=Gray]*THUMB*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=79][Content=Are you okay?]]
+[Choice2=[NextScene=79][Content=What was that?!]]
+]
 ]</v>
       </c>
     </row>
@@ -12340,9 +13246,11 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="F80" s="8"/>
+        <v>389</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>554</v>
+      </c>
       <c r="G80" s="23" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=79
@@ -12352,6 +13260,9 @@
 OH SHIT, WHY AM I ON A PILE OF CORPSES?[Wait=500] WHY WOULD YOU MAKE A ROOM FILLED WITH DEAD CLONES?![Wait=500][Space=2]
 [Color=Gray]*Mechanical noises*[Color=White]...[Wait=500] What was that noise?... WHY ARE THE WALLS GETTING TIGHTER?![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=80][Content=Climb back to the vent!]]
+]
 ]</v>
       </c>
     </row>
@@ -12363,9 +13274,11 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="F81" s="8"/>
+        <v>390</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>555</v>
+      </c>
       <c r="G81" s="23" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=80
@@ -12375,6 +13288,10 @@
 I don't want to die here![Wait=500] I don't want to die as a vulgar piece of meat![Wait=500] PLEASE HELP ME![Wait=500][Space=2]
 STOP THIS NOW!!![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=81][TrustAdd=-25][Content=I can't do anything!]]
+[Choice2=[NextScene=81][TrustAdd=-25][Content=You're the one who jumped in the lion's den!]]
+]
 ]</v>
       </c>
     </row>
@@ -12388,9 +13305,11 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="F82" s="8"/>
+        <v>391</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>558</v>
+      </c>
       <c r="G82" s="23" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=81
@@ -12401,6 +13320,11 @@
 [Color=Gray]*Crushing noises intensifies*[Color=White]...[Wait=500] I hope you're happy now that you can hear me die crushed alive.[Wait=500][Space=2]
 You did this with all of the other clones huh?[Wait=500] Hearing them die on live.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=82][TrustAdd=-25][Content=GET OUT OF HERE!]]
+[Choice2=[NextScene=82][TrustAdd=-25][Content=I DIDN'T DO ANYTHING, I SWEAR!]]
+[Choice3=[NextScene=82][TrustAdd=-25][Content=That's for not believing me!]]
+]
 ]</v>
       </c>
     </row>
@@ -12414,9 +13338,11 @@
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>397</v>
-      </c>
-      <c r="F83" s="13"/>
+        <v>392</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>556</v>
+      </c>
       <c r="G83" s="24" t="str">
         <f t="shared" si="3"/>
         <v>[Scene=82
@@ -12428,6 +13354,10 @@
 FUCK Y-[Color=Gray]*Crush*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=83][TrustAdd=-25][Content=Oh no...]]
+[Choice2=[NextScene=83][TrustAdd=-25][Content=That's what you deserved.]]
+]
 ]</v>
       </c>
     </row>
@@ -12441,9 +13371,11 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="F84" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G84" s="23" t="str">
         <f t="shared" ref="G84:G92" si="4">"[Scene=" &amp; A84 &amp; IF(OR(B84&lt;&gt;"",C84&lt;&gt;"",D84&lt;&gt;""),CHAR(10),"") &amp; IF(B84&lt;&gt;"","[BeepBack=" &amp; B84 &amp; "]","") &amp; IF(C84&lt;&gt;"","[Connection=" &amp; C84 &amp; "]","") &amp; IF(D84&lt;&gt;"","[Timer=" &amp; D84 &amp; "]","") &amp; IF(E84&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E84 &amp; CHAR(10) &amp; "]","") &amp; IF(F84&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F84 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=83
@@ -12454,6 +13386,12 @@
 [Color=Red]{THEY WERE MADE USING THEIR PAST SELVES. AND NOW IT'S THEIR TURN?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -12465,9 +13403,11 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="F85" s="8"/>
+        <v>394</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>557</v>
+      </c>
       <c r="G85" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=84
@@ -12475,6 +13415,9 @@
 I... It can't be.[Wait=500] I'm like them?[Wait=500] I'm also a clone?[Wait=500][Space=2]
 B-But...[Wait=500] No, that makes sense after all.[Wait=500][Space=2]
 Your voice, it striked me at first but I considered it was a coincidence.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=85][Content=My voice? What about it?]]
 ]
 ]</v>
       </c>
@@ -12487,9 +13430,11 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="F86" s="8"/>
+        <v>395</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>559</v>
+      </c>
       <c r="G86" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=85
@@ -12497,6 +13442,11 @@
 It's the same as mine! You're me!...[Wait=500][Space=2]
 No...[Wait=500] It's not that...[Wait=500][Space=2]
 I'M YOU![Wait=500] I'M A COPY OF YOU![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=86][Content=What's your theory?]]
+[Choice2=[NextScene=86][TrustAdd=-25][Content=Have you become insane?]]
+[Choice3=[NextScene=86][TrustAdd=25][Content=You might be right about that...]]
 ]
 ]</v>
       </c>
@@ -12509,9 +13459,11 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="F87" s="8"/>
+        <v>396</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>560</v>
+      </c>
       <c r="G87" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=86
@@ -12519,6 +13471,10 @@
 Doesn't it make sense for you?[Wait=500] Why would I contact you in the first place?[Wait=500] BECAUSE YOU'RE THE ORIGINAL![Wait=500][Space=2]
 All of these copies, they never called you right?[Wait=500] They look dismorphed, they are failed versions![Wait=500][Space=2]
 Then it means I am somewhat special compared to others. I am a successful clone...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=87][Content=Is there anything more clues here?]]
+[Choice2=[NextScene=90][Content=I don't care about who you are, LET'S GET OUT!]]
 ]
 ]</v>
       </c>
@@ -12531,9 +13487,11 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="F88" s="8"/>
+        <v>397</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>561</v>
+      </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=87
@@ -12543,6 +13501,10 @@
 It says here that...[Wait=500][Space=2]
 "The faulty subjects are disposed in the nutrients grinder so they can be recycled as energy for the future subjects conception.".[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=88][Content=Nutrient grinder?]]
+[Choice2=[NextScene=89][Content=Does that mean they might be other like us in here?]]
+]
 ]</v>
       </c>
     </row>
@@ -12554,9 +13516,11 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="F89" s="8"/>
+        <v>398</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>562</v>
+      </c>
       <c r="G89" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=88
@@ -12564,6 +13528,10 @@
 The plan shows what seems to be an gigantic hydraulic press.[Wait=500][Space=2]
 T-They put all of the clones here and the flesh and blood is transferred into...[Wait=500][Space=2]
 Into what seems to be cloning capsules...[Wait=500] All this diagram forms a loop.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=89][Content=So all of these dead bodies are... me?]]
+[Choice2=[NextScene=89][Content=But what about the monster from before. Was it a clone?]]
 ]
 ]</v>
       </c>
@@ -12576,9 +13544,11 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="F90" s="8"/>
+        <v>399</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>563</v>
+      </c>
       <c r="G90" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=89
@@ -12588,6 +13558,9 @@
 There's a fuse protected under a cloche![Wait=500] "Only use for emergency escape"[Wait=500][Space=2]
 IT'S FOR THE TRAPDOOR FROM BEFORE![Wait=500] I CAN FINALLY GET OUT![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=90][Content=Is there a way to go back at the surface?]]
+]
 ]</v>
       </c>
     </row>
@@ -12599,9 +13572,11 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="F91" s="8"/>
+        <v>400</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>564</v>
+      </c>
       <c r="G91" s="23" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=90
@@ -12612,6 +13587,10 @@
 Now that I'm back at this vivarium, I just have to remember my way ba-...[Wait=500][Space=2]
 .[Wait=500].[Wait=500].[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=91][Content=What's up? Why did you stop talking?]]
+[Choice1=[NextScene=91][Content=Hello? You're there?]]
+]
 ]</v>
       </c>
     </row>
@@ -12623,9 +13602,11 @@
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>406</v>
-      </c>
-      <c r="F92" s="13"/>
+        <v>401</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>565</v>
+      </c>
       <c r="G92" s="24" t="str">
         <f t="shared" si="4"/>
         <v>[Scene=91
@@ -12636,6 +13617,9 @@
 It's looking at me...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=92][Content=Don't move.]]
+]
 ]</v>
       </c>
     </row>
@@ -12651,9 +13635,11 @@
         <v>10</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="F93" s="8"/>
+        <v>402</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>567</v>
+      </c>
       <c r="G93" s="23" t="str">
         <f t="shared" ref="G93:G135" si="5">"[Scene=" &amp; A93 &amp; IF(OR(B93&lt;&gt;"",C93&lt;&gt;"",D93&lt;&gt;""),CHAR(10),"") &amp; IF(B93&lt;&gt;"","[BeepBack=" &amp; B93 &amp; "]","") &amp; IF(C93&lt;&gt;"","[Connection=" &amp; C93 &amp; "]","") &amp; IF(D93&lt;&gt;"","[Timer=" &amp; D93 &amp; "]","") &amp; IF(E93&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E93 &amp; CHAR(10) &amp; "]","") &amp; IF(F93&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F93 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=92
@@ -12664,6 +13650,12 @@
 WHAT IS THE WAY BACK TO THE ENTRANCE?!!![Wait=500][Space=2]
 [Color=Magenta][Beep=True]ReMeM[Wait=500][Beep=True]beR yOuR[Wait=500][Beep=True]  pAtH tO[Wait=500][Beep=True]  tHe ViVa[Wait=500][Beep=True]rIuM,[Wait=500][Beep=True]  bUt bAc[Wait=500][Beep=True]kWaRdS![Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=93][Content=GO EAST!]]
+[Choice3=[NextScene=100][Content=GO SOUTH!]]
+[Choice4=[NextScene=100][Content=GO WEST!]]
+]
 ]</v>
       </c>
     </row>
@@ -12677,9 +13669,11 @@
         <v>10</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="F94" s="8"/>
+        <v>403</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>568</v>
+      </c>
       <c r="G94" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=93
@@ -12689,6 +13683,12 @@
 huff...[Wait=500] huff...[Wait=500][Space=2]
 I CAN HEAR ME RUNNING BEHIND ME, WHAT WAS IT NEXT?!![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=100][Content=GO EAST!]]
+[Choice3=[NextScene=94][Content=GO SOUTH!]]
+[Choice4=[NextScene=100][Content=GO WEST!]]
+]
 ]</v>
       </c>
     </row>
@@ -12702,9 +13702,11 @@
         <v>10</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="F95" s="8"/>
+        <v>404</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>569</v>
+      </c>
       <c r="G95" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=94
@@ -12716,6 +13718,12 @@
 FUCK FUCK FUCK IT'S GETTING CLOSER, BUT I THINK I'M ON THE RIGHT WAY![Wait=500][Space=2]
 WHAT WAS IT LAST?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[Default=True][NextScene=100][Content=GO NORTH!]]
+[Choice2=[NextScene=100][Content=GO EAST!]]
+[Choice3=[NextScene=100][Content=GO SOUTH!]]
+[Choice4=[NextScene=95][Content=GO WEST!]]
+]
 ]</v>
       </c>
     </row>
@@ -12729,9 +13737,11 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="F96" s="8"/>
+        <v>405</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>570</v>
+      </c>
       <c r="G96" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=95
@@ -12743,6 +13753,10 @@
 [Color=Gray]*Metallic rumbling*[Color=White]... [Color=Gray]*CLANG*[Color=White]...[Wait=500][Space=2]
 ...[Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=96][Content=HURRY!]]
+[Choice2=[NextScene=96][Content=DID IT WORKED?]]
+]
 ]</v>
       </c>
     </row>
@@ -12754,9 +13768,11 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="F97" s="8"/>
+        <v>406</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>571</v>
+      </c>
       <c r="G97" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=96
@@ -12766,6 +13782,10 @@
 ...[Wait=500] I ran so much that I'm back at the trapdoor now...[Wait=500][Space=2]
 So...[Wait=500] I just have to put the fuse here and...[Wait=500][Beep=True] [Color=Gray]*Mechanical beeping*[Color=White]... YEEES![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=97][Content=It opened?]]
+[Choice2=[NextScene=97][Content=IT OPENED!]]
+]
 ]</v>
       </c>
     </row>
@@ -12779,9 +13799,11 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="F98" s="8"/>
+        <v>407</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>572</v>
+      </c>
       <c r="G98" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=97
@@ -12791,6 +13813,9 @@
 There are stairs here.[Wait=500] I'm getting down there.[Wait=500][Space=2]
 ...Oh my god...[Wait=500] It was such an intens-[Color=Gray]*SHKRRRRRRRRR*[Color=White]...[Wait=500] I'm so happy that you were here to help me.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=98][Content=Wait, the signal's getting weaker!]]
+]
 ]</v>
       </c>
     </row>
@@ -12804,9 +13829,11 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="F99" s="8"/>
+        <v>408</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>573</v>
+      </c>
       <c r="G99" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=98
@@ -12817,6 +13844,9 @@
 ...It was a pleasu-[Color=Gray]*SHKRRRRRRRRRRRRRRR*[Color=White]...[Wait=500] Thank you, I'm glad to be y-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 Goodbye...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=99][Content=I hope you'll be safe. Goodbye.]]
+]
 ]</v>
       </c>
     </row>
@@ -12830,9 +13860,11 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="F100" s="8"/>
+        <v>409</v>
+      </c>
+      <c r="F100" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=99
@@ -12843,6 +13875,12 @@
 [Color=Green]{ONE LIFE SAVED, BUT WHAT ABOUT THE OTHERS?}[Color=White][Wait=500][Space=2]
 [Color=Green]GOOD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -12856,9 +13894,11 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="F101" s="8"/>
+        <v>411</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>574</v>
+      </c>
       <c r="G101" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=100
@@ -12870,6 +13910,9 @@
 Wait, wait, wait, wait...[Wait=500] No please don't hurt me...[Wait=500] We're the same, we can escape together![Wait=500][Space=2]
 [Color=Cyan]IT'S ALL BECAUSE HE WAS WAITING FOR YOU THAT HE MADE ME![Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=101][Content=W-What is he talking about?]]
+]
 ]</v>
       </c>
     </row>
@@ -12883,9 +13926,11 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="F102" s="8"/>
+        <v>412</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>575</v>
+      </c>
       <c r="G102" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=101
@@ -12896,6 +13941,9 @@
 Oh no, NO PLEA-urk!...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=102][Content=...]]
+]
 ]</v>
       </c>
     </row>
@@ -12909,9 +13957,11 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="F103" s="8"/>
+        <v>410</v>
+      </c>
+      <c r="F103" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G103" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=102
@@ -12922,6 +13972,12 @@
 [Color=Red]{YOU GOT TOO CLOSE OF AN INFECTED ONE. IS THERE MAYBE ANOTHER WAY?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -12933,9 +13989,11 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="F104" s="8"/>
+        <v>413</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>576</v>
+      </c>
       <c r="G104" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=103
@@ -12943,6 +14001,10 @@
 I'M RUNNING AS FAST AS I CAN BUT-[Color=Gray]*Rumbling noises*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 Fuck...[Wait=500] The tunnel collapsed behind me.[Wait=500] This thing must have been crushed by the roof...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=104][Content=Where are you now?]]
+[Choice2=[NextScene=105][TrustAdd=25][Content=Are you safe?]]
 ]
 ]</v>
       </c>
@@ -12955,9 +14017,11 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="F105" s="8"/>
+        <v>415</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>577</v>
+      </c>
       <c r="G105" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=104
@@ -12967,6 +14031,11 @@
 Wait for me to process everything that's going on, Jesus![Wait=500][Space=2]
 I just been chased by a disfigured human for god sake![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=106][Content=Disfigured human?]]
+[Choice2=[NextScene=107][TrustAdd=25][Content=Right, take your time to breath.]]
+[Choice3=[NextScene=108][TrustAdd=-25][Content=I didn't know you were a soft belly.]]
+]
 ]</v>
       </c>
     </row>
@@ -12978,9 +14047,11 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="F106" s="8"/>
+        <v>414</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>578</v>
+      </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=105
@@ -12988,6 +14059,9 @@
 Y-Yeah...[Wait=500] Thanks for asking.[Wait=500][Space=2]
 I'm in a corridor now, and it seems far more preserved than annything I saw on this island before.[Wait=500][Space=2]
 The lights are even working in here.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]
 ]
 ]</v>
       </c>
@@ -13000,9 +14074,11 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="F107" s="8"/>
+        <v>416</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>579</v>
+      </c>
       <c r="G107" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=106
@@ -13010,6 +14086,10 @@
 That's right.[Wait=500] I turned my back for a blink of a second and I saw what this monster was.[Wait=500][Space=2]
 It was a human, as tall as I am, but with a deformed face.[Wait=500][Space=2]
 ...[Wait=500] It was horrifying. I wish I never saw that.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=109][TrustAdd=-25][Content=Why did it chase you in the first place?]]
+[Choice2=[NextScene=110][Content=It might be better to get out of here since it might get out of the rubble.]]
 ]
 ]</v>
       </c>
@@ -13022,9 +14102,11 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="F108" s="8"/>
+        <v>417</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>580</v>
+      </c>
       <c r="G108" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=107
@@ -13034,6 +14116,9 @@
 Ah shit, that was not the best idea to take a huge breath near a pile of freshly collapsed tunnels.[Wait=500][Space=2]
 [Color=Gray]*Cough*[Color=White]...[Wait=500] But thanks for the attention anyway, I'm ready to go now.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=111][Content=Can you describe what's around you?]]
+]
 ]</v>
       </c>
     </row>
@@ -13045,9 +14130,11 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="8" t="s">
-        <v>423</v>
-      </c>
-      <c r="F109" s="8"/>
+        <v>418</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>578</v>
+      </c>
       <c r="G109" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=108
@@ -13057,6 +14144,9 @@
 To change the subject, I'm now in a corridor now, and it seems far more preserved than annything I saw on this island before.[Wait=500][Space=2]
 The lights are even working in here.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]
+]
 ]</v>
       </c>
     </row>
@@ -13068,9 +14158,11 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="F110" s="8"/>
+        <v>419</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>578</v>
+      </c>
       <c r="G110" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=109
@@ -13082,6 +14174,9 @@
 Anyway.[Wait=500] I 'm in front of a corridor, and it seems far more preserved than annything I saw on this island.[Wait=500][Space=2]
 The lights are even working in here.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]
+]
 ]</v>
       </c>
     </row>
@@ -13093,9 +14188,11 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="F111" s="8"/>
+        <v>420</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>578</v>
+      </c>
       <c r="G111" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=110
@@ -13105,6 +14202,9 @@
 I'm now inside a corridor, and it seems far more preserved than annything I saw on this island before.[Wait=500][Space=2]
 The lights are even working in here.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]
+]
 ]</v>
       </c>
     </row>
@@ -13116,9 +14216,11 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="F112" s="8"/>
+        <v>421</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>578</v>
+      </c>
       <c r="G112" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=111
@@ -13126,6 +14228,9 @@
 Of course! I'm in front of a corridor.[Wait=500][Space=2]
 It seems far more preserved than annything I saw on this island before.[Wait=500][Space=2]
 The lights are even working in here.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=112][Content=Doesn't it seems like an inhabited place?]]
 ]
 ]</v>
       </c>
@@ -13138,9 +14243,11 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="F113" s="8"/>
+        <v>422</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>600</v>
+      </c>
       <c r="G113" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=112
@@ -13148,6 +14255,10 @@
 Yes.[Wait=500][Space=2]
 I've didn't meet any working light before.[Wait=500] The only thing that was working was this escalator from before.[Wait=500][Space=2]
 It seems that I'm heading to a new place designed for me by the one who brought me here.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=113][Content=It might be another trap then, can't you go back?]]
+[Choice2=[NextScene=114][Content=It's time to face another test it seems.]]
 ]
 ]</v>
       </c>
@@ -13160,9 +14271,11 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="F114" s="8"/>
+        <v>423</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>581</v>
+      </c>
       <c r="G114" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=113
@@ -13173,6 +14286,9 @@
 [Color=Gray]*Footsteps echoing*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500] I can't believe it.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=115][Content=You can't believe what?]]
+]
 ]</v>
       </c>
     </row>
@@ -13184,9 +14300,11 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="F115" s="8"/>
+        <v>424</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>581</v>
+      </c>
       <c r="G115" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=114
@@ -13196,6 +14314,9 @@
 [Color=Gray]*Footsteps echoing*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500] I can't believe it.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=115][Content=You can't believe what?]]
+]
 ]</v>
       </c>
     </row>
@@ -13207,9 +14328,11 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="F116" s="8"/>
+        <v>425</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>582</v>
+      </c>
       <c r="G116" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=115
@@ -13217,6 +14340,10 @@
 Th-THERE'S A BOAT HERE![Wait=500] It's put on the water, ready to be used![Wait=500][Space=2]
 There's even a hole leading outside, I can see the sunshine from here![Wait=500][Space=2]
 I'M FINALLY FREE![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=116][Content=Not so fast, it might be a trap!]]
+[Choice1=[NextScene=117][Content=What kind of boat is it?]]
 ]
 ]</v>
       </c>
@@ -13229,15 +14356,20 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="F117" s="8"/>
+        <v>426</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>583</v>
+      </c>
       <c r="G117" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=116
 [Content=
 What do you mean it's a trap?[Wait=500] THE BOAT'S RIGHT HERE![Wait=500][Space=2]
 I just have to get on it and I'll finally be free AHAHAHAHAH!!!![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=118][Content=Focus now! Is there nothing else in this room?]]
 ]
 ]</v>
       </c>
@@ -13250,15 +14382,20 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="F118" s="8"/>
+        <v>427</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>584</v>
+      </c>
       <c r="G118" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=117
 [Content=
 A YACHT![Wait=500] I'M GOING TO ESCAPE FROM THIS NIGHTMARE ISLAND ON A YACHT![Wait=500][Space=2]
 YAHOOOOOO!!![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=118][NextSceneNoTrust=130][TrustNeed=50][Content=Focus now! Is there nothing else in this room?]]
 ]
 ]</v>
       </c>
@@ -13271,9 +14408,11 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="F119" s="8"/>
+        <v>428</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>585</v>
+      </c>
       <c r="G119" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=118
@@ -13283,6 +14422,11 @@
 ...[Wait=500] Wait...[Wait=500] Is that someone standing on the dock?[Wait=500][Space=2]
 It's not the monster from before.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=119][Content=Try to-...]]
+[Choice2=[NextScene=119][Content=Go in-...]]
+[Choice3=[NextScene=119][Content=Hide from-...]]
+]
 ]</v>
       </c>
     </row>
@@ -13294,9 +14438,11 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="F120" s="8"/>
+        <v>430</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>586</v>
+      </c>
       <c r="G120" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=119
@@ -13304,6 +14450,10 @@
 [Color=Yellow]I didn't expected you there, to be honest. This place was supposed to be hidden from you.[Color=White][Wait=500][Space=2]
 W-What? Who are you?[Wait=500][Space=2]
 [Color=Yellow]I'm your creator. And the one you're talking to with that phone is the original.[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=120][Content=Original? What does he mean?]]
+[Choice2=[NextScene=120][Content=What do you mean by creator?]]
 ]
 ]</v>
       </c>
@@ -13316,9 +14466,11 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="F121" s="8"/>
+        <v>431</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>587</v>
+      </c>
       <c r="G121" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=120
@@ -13328,6 +14480,10 @@
 [Color=Yellow]He resisted and still remains unaffected by the thing that transformed the thing that followed you before.[Color=White][Wait=500][Space=2]
 W-Wait...[Wait=500] What do you mean by clone?[Wait=500] I have feelings! I can feel pain![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=121][Content=I...]]
+[Choice2=[NextScene=121][Content=But...]]
+]
 ]</v>
       </c>
     </row>
@@ -13339,9 +14495,11 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="F122" s="8"/>
+        <v>432</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>588</v>
+      </c>
       <c r="G122" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=121
@@ -13351,6 +14509,9 @@
 [Color=Yellow]Confused, right?[Wait=500] just come to me and accept what you're supposed to be, a succesful vessel.[Color=White][Wait=500][Space=2]
 [Color=Yellow]Your blood will save millions, let me just exctract all of it from you![Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=122][Content=HE'S GOING TO KILL YOU!]]
+]
 ]</v>
       </c>
     </row>
@@ -13362,9 +14523,11 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="F123" s="8"/>
+        <v>433</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>589</v>
+      </c>
       <c r="G123" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=122
@@ -13374,6 +14537,9 @@
 [Color=Yellow]Resisting, uh?[Wait=500] Looks like I'll have to do the job myself.[Color=White][Wait=500][Space=2]
 What do you mea-OH MY GOD HE HAS A GUN![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=123][TrustAdd=25][Content=FIGHT HIM!]]
+]
 ]</v>
       </c>
     </row>
@@ -13385,9 +14551,11 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="F124" s="8"/>
+        <v>434</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>590</v>
+      </c>
       <c r="G124" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=123
@@ -13398,6 +14566,9 @@
 [Color=Yellow]Stay still you insignificant piece of flesh![Color=White][Wait=500][Space=2]
 NO WAY![Wait=500] I'M COMING FOR YOU![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=124][TrustAdd=25][Content=GIVE HIM WHAT HE DESERVES!]]
+]
 ]</v>
       </c>
     </row>
@@ -13409,9 +14580,11 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="F125" s="8"/>
+        <v>435</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>591</v>
+      </c>
       <c r="G125" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=124
@@ -13422,6 +14595,9 @@
 Well, it's only fair that I take your life for the many that you took.[Wait=500][Space=2]
 [Color=Gray]*WHAM*[Color=White]...[Wait=500] [Color=Gray]*Splash*[Color=White]...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=125][Content=You killed him?]]
+]
 ]</v>
       </c>
     </row>
@@ -13433,9 +14609,11 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="F126" s="8"/>
+        <v>436</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>592</v>
+      </c>
       <c r="G126" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=125
@@ -13443,6 +14621,9 @@
 ...[Wait=500][Space=2]
 ...[Wait=500] Well, his body is face down in the water, and it doesn't seem to care so I'll assume he is.[Wait=500][Space=2]
 To be honnest, that was the best punch I gave to someone in my entire life...[Wait=500] since it was the first.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=126][Content=What are you going to do now?]]
 ]
 ]</v>
       </c>
@@ -13455,9 +14636,11 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="F127" s="8"/>
+        <v>437</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>593</v>
+      </c>
       <c r="G127" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=126
@@ -13465,6 +14648,9 @@
 I'm heading to the boat.[Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] Yeah, I called it, it's his personnal boat.[Wait=500][Space=2]
 There is enough rations to live on the sea for a month.[Wait=500] Seems like I'm escaping for good now![Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=127][Content=I hope you'll have a good trip on the sea!]]
 ]
 ]</v>
       </c>
@@ -13477,9 +14663,11 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="F128" s="8"/>
+        <v>438</v>
+      </c>
+      <c r="F128" s="8" t="s">
+        <v>594</v>
+      </c>
       <c r="G128" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=127
@@ -13489,6 +14677,9 @@
 We could maybe meet one day, but I feel like starting a new life, creating my own new identity.[Wait=500][Space=2]
 But who knows?[Wait=500] Maybe we'll meet again.[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=128][Content=Well then, I guess it's a goodbye.]]
+]
 ]</v>
       </c>
     </row>
@@ -13502,9 +14693,11 @@
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="F129" s="8"/>
+        <v>439</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>595</v>
+      </c>
       <c r="G129" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=128
@@ -13515,6 +14708,9 @@
 I'll be heading north, I hope to find civilization quick.[Wait=500][Space=2]
 I'll let you hang up, my hands are pretty taken by the steering wheel ahah![Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=129][Content=See you around.]]
+]
 ]</v>
       </c>
     </row>
@@ -13528,9 +14724,11 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="F130" s="8"/>
+        <v>440</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G130" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=129
@@ -13541,6 +14739,12 @@
 [Color=Green]{THE MONSTER IS GONE, THE SCIENTIST TOO, BUT WHAT DID THEY SEEK?}[Color=White][Wait=500][Space=2]
 [Color=Green]GOOD ENDING.[Color=White][Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
+]
 ]</v>
       </c>
     </row>
@@ -13552,15 +14756,20 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="F131" s="8"/>
+        <v>441</v>
+      </c>
+      <c r="F131" s="8" t="s">
+        <v>596</v>
+      </c>
       <c r="G131" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=130
 [Content=
 I don't care about your "check this, check that" now.[Wait=500] I'M FREE TO GO![Wait=500][Space=2]
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] Soooo... How does this engine works?[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=131][Content=You want me to search on the internet?]]
 ]
 ]</v>
       </c>
@@ -13573,9 +14782,11 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="F132" s="8"/>
+        <v>442</v>
+      </c>
+      <c r="F132" s="8" t="s">
+        <v>597</v>
+      </c>
       <c r="G132" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=131
@@ -13583,6 +14794,9 @@
 Oh come on![Wait=500] I don't need that anymore![Wait=500][Space=2]
 I'M FREE-[Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
 [Color=Yellow]You thought you could escape me, huh?[Wait=500] Well too bad, but I'm going to have to replace you.[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=132][Content=Who is talking?]]
 ]
 ]</v>
       </c>
@@ -13595,9 +14809,11 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="F133" s="8"/>
+        <v>443</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>598</v>
+      </c>
       <c r="G133" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=132
@@ -13607,6 +14823,9 @@
 [Color=Yellow]Now...[Wait=500] You got out of the path I made for you thanks to incredible odds, but that's the end of it.[Color=White][Wait=500][Space=2]
 W-What do you mean?[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=133][Content=FIGHT BACK, DO SOMETHING!]]
+]
 ]</v>
       </c>
     </row>
@@ -13620,9 +14839,11 @@
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8" t="s">
-        <v>449</v>
-      </c>
-      <c r="F134" s="8"/>
+        <v>444</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>599</v>
+      </c>
       <c r="G134" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=133
@@ -13634,6 +14855,9 @@
 Don't tell me you-[Color=Gray]*BANG*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 ]
+[Choices=
+[Choice1=[NextScene=134][Content=No... It can't be...]]
+]
 ]</v>
       </c>
     </row>
@@ -13647,9 +14871,11 @@
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="F135" s="8"/>
+        <v>445</v>
+      </c>
+      <c r="F135" s="8" t="s">
+        <v>517</v>
+      </c>
       <c r="G135" s="23" t="str">
         <f t="shared" si="5"/>
         <v>[Scene=134
@@ -13661,6 +14887,12 @@
 [Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
 [Color=Red]{HE CAUGHT HIM. WAS THERE NO OTHER CHOICE?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextChapter=3][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]
 ]
 ]</v>
       </c>

</xml_diff>

<commit_message>
Fix: Chapter 3 Corrections
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2026\C++\Signal_Lost\Signal_Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEED3834-5C51-496A-AFF2-EA5226E1397E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EF9BF9-3CA0-4700-86EC-627CC9E8AEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters_Header" sheetId="3" r:id="rId1"/>
@@ -1850,12 +1850,6 @@
 ...[Wait=500] It seems that it comes from behind this one rusty door.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I-...[Wait=500] I DON'T FREAKING KNOW![Wait=500][Space=2]_
-THEY ARE PILES OF DEAD BODIES AND YOU THINK THE FIRST QUESTIONS THAT COMES TO MY MIND IS![Wait=500][Space=2]
-"Oh! Why did they landed here? Did they die of pneumonia? How curious!"[Wait=500]...[Wait=500][Space=2]
-NO, I'M SCARED, I WANT TO GET OUT OF HERE![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Their face.[Wait=500] They look dismorphed...[Wait=500][Space=2]
 ...W-What?...[Wait=500] It's impossible...[Wait=500][Space=2]
 ...[Wait=500] Why do they have the same clothes, the same body traits as...[Wait=500] me?[Wait=500] WHY DO THEY LOOK LIKE ME?![Wait=500][Space=2]
@@ -2613,9 +2607,6 @@
     <t>[Choice1=[NextScene=54][Content=What did it look like?]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=54][Content=We'll get you out of here by moving forward.]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=56][Content=You're under the island! Maybe you can access other parts of the city from here.]]</t>
   </si>
   <si>
@@ -2925,6 +2916,15 @@
 ...[Wait=500][Space=2]
 ...[Wait=500] [Color=Gray]*Vomit noises*[Color=White]...[Wait=500][Space=2]
 OH MY-[Color=Gray]*Cough*[Color=White]... [Color=Gray]*Cough*[Color=White]...[Wait=500] THERE ARE DEAD CORPSES ALL OVER THE GROUND![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I-...[Wait=500] I DON'T FREAKING KNOW![Wait=500][Space=2]_
+THEY ARE PILES OF DEAD BODIES AND YOU THINK THE FIRST QUESTIONS THAT COMES TO MY MIND IS![Wait=500][Space=2]
+"Oh! Why did they landed here?"[Wait=500] "Did they die of pneumonia?"[Wait=500] "How curious!"...[Wait=500][Space=2]
+NO, I'M SCARED, I WANT TO GET OUT OF HERE![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=55][Content=We'll get you out of here by moving forward.]]</t>
   </si>
 </sst>
 </file>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
@@ -6046,7 +6046,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>34</v>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>50</v>
@@ -6406,7 +6406,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>51</v>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>59</v>
@@ -6796,7 +6796,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>63</v>
@@ -6883,7 +6883,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>42</v>
@@ -6940,7 +6940,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>65</v>
@@ -6968,7 +6968,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>66</v>
@@ -6996,7 +6996,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>67</v>
@@ -7025,7 +7025,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>68</v>
@@ -7082,7 +7082,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>69</v>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>45</v>
@@ -7442,7 +7442,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>75</v>
@@ -7497,7 +7497,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>77</v>
@@ -7702,7 +7702,7 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>84</v>
@@ -7788,8 +7788,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView topLeftCell="E106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8029,7 +8029,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>291</v>
@@ -8057,7 +8057,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>159</v>
@@ -8196,7 +8196,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>294</v>
@@ -8449,7 +8449,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>300</v>
@@ -8503,7 +8503,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>300</v>
@@ -8669,7 +8669,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>305</v>
@@ -8753,7 +8753,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>164</v>
@@ -8868,7 +8868,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>168</v>
@@ -9117,7 +9117,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>173</v>
@@ -9183,7 +9183,7 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>175</v>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>176</v>
@@ -9279,7 +9279,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>179</v>
@@ -9610,7 +9610,7 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>186</v>
@@ -9639,7 +9639,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>310</v>
@@ -9667,7 +9667,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>187</v>
@@ -9865,7 +9865,7 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>194</v>
@@ -9949,7 +9949,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>196</v>
@@ -10029,7 +10029,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>198</v>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>311</v>
@@ -10440,7 +10440,7 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>210</v>
@@ -10862,7 +10862,7 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F108" s="13" t="s">
         <v>177</v>
@@ -10927,8 +10927,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView topLeftCell="E55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10977,7 +10977,7 @@
         <v>316</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -11005,7 +11005,7 @@
         <v>317</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11035,7 +11035,7 @@
         <v>318</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11061,7 +11061,7 @@
         <v>319</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11092,7 +11092,7 @@
         <v>320</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11121,7 +11121,7 @@
         <v>321</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11151,7 +11151,7 @@
         <v>322</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11181,7 +11181,7 @@
         <v>323</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11210,7 +11210,7 @@
         <v>324</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11242,7 +11242,7 @@
         <v>325</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11269,7 +11269,7 @@
         <v>326</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11297,7 +11297,7 @@
         <v>327</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11324,7 +11324,7 @@
         <v>328</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11351,7 +11351,7 @@
         <v>329</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11377,7 +11377,7 @@
         <v>330</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11404,10 +11404,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11437,7 +11437,7 @@
         <v>331</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11467,7 +11467,7 @@
         <v>332</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11493,7 +11493,7 @@
         <v>333</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11522,7 +11522,7 @@
         <v>334</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11548,7 +11548,7 @@
         <v>335</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11578,7 +11578,7 @@
         <v>336</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11609,7 +11609,7 @@
         <v>337</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11641,7 +11641,7 @@
         <v>338</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11670,7 +11670,7 @@
         <v>339</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11700,7 +11700,7 @@
         <v>340</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11731,7 +11731,7 @@
         <v>341</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11759,7 +11759,7 @@
         <v>342</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11788,7 +11788,7 @@
         <v>343</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11817,7 +11817,7 @@
         <v>344</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11846,7 +11846,7 @@
         <v>345</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11874,7 +11874,7 @@
         <v>350</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11903,7 +11903,7 @@
         <v>346</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -11931,7 +11931,7 @@
         <v>347</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
@@ -11958,7 +11958,7 @@
         <v>348</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -11984,10 +11984,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12015,7 +12015,7 @@
         <v>349</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12043,10 +12043,10 @@
         <v>60</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12079,7 +12079,7 @@
         <v>351</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12112,7 +12112,7 @@
         <v>352</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12149,7 +12149,7 @@
         <v>353</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12180,7 +12180,7 @@
         <v>354</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12209,7 +12209,7 @@
         <v>355</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12234,10 +12234,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12267,7 +12267,7 @@
         <v>356</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12294,7 +12294,7 @@
         <v>357</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12323,7 +12323,7 @@
         <v>358</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12350,7 +12350,7 @@
         <v>359</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12386,7 +12386,7 @@
         <v>360</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12415,7 +12415,7 @@
         <v>361</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12441,7 +12441,7 @@
         <v>362</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12470,7 +12470,7 @@
         <v>363</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12500,7 +12500,7 @@
         <v>364</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12527,7 +12527,7 @@
         <v>365</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>529</v>
+        <v>608</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12538,7 +12538,7 @@
 ...[Wait=500] Why can’t I wake up from this nightmare?[Wait=500][Space=2]
 ]
 [Choices=
-[Choice1=[NextScene=54][Content=We'll get you out of here by moving forward.]]
+[Choice1=[NextScene=55][Content=We'll get you out of here by moving forward.]]
 ]
 ]</v>
       </c>
@@ -12554,7 +12554,7 @@
         <v>366</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12581,7 +12581,7 @@
         <v>367</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12608,7 +12608,7 @@
         <v>368</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12635,7 +12635,7 @@
         <v>369</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12666,7 +12666,7 @@
         <v>370</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12695,7 +12695,7 @@
         <v>371</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12723,7 +12723,7 @@
         <v>372</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12753,7 +12753,7 @@
         <v>373</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12782,7 +12782,7 @@
         <v>374</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12810,7 +12810,7 @@
         <v>375</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12842,7 +12842,7 @@
         <v>376</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G74" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -12876,7 +12876,7 @@
         <v>377</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
@@ -12908,7 +12908,7 @@
         <v>378</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -12939,7 +12939,7 @@
         <v>379</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
@@ -12967,7 +12967,7 @@
         <v>380</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
@@ -12994,7 +12994,7 @@
         <v>381</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13020,10 +13020,10 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13050,10 +13050,10 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>382</v>
+        <v>607</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13061,7 +13061,7 @@
 [Content=
 I-...[Wait=500] I DON'T FREAKING KNOW![Wait=500][Space=2]_
 THEY ARE PILES OF DEAD BODIES AND YOU THINK THE FIRST QUESTIONS THAT COMES TO MY MIND IS![Wait=500][Space=2]
-"Oh! Why did they landed here? Did they die of pneumonia? How curious!"[Wait=500]...[Wait=500][Space=2]
+"Oh! Why did they landed here?"[Wait=500] "Did they die of pneumonia?"[Wait=500] "How curious!"...[Wait=500][Space=2]
 NO, I'M SCARED, I WANT TO GET OUT OF HERE![Wait=500][Space=2]
 ]
 [Choices=
@@ -13079,10 +13079,10 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="G74" s="24" t="str">
         <f t="shared" si="2"/>
@@ -13107,10 +13107,10 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G75" s="23" t="str">
         <f>"[Scene=" &amp; A75 &amp; IF(OR(B75&lt;&gt;"",C75&lt;&gt;"",D75&lt;&gt;""),CHAR(10),"") &amp; IF(B75&lt;&gt;"","[BeepBack=" &amp; B75 &amp; "]","") &amp; IF(C75&lt;&gt;"","[Connection=" &amp; C75 &amp; "]","") &amp; IF(D75&lt;&gt;"","[Timer=" &amp; D75 &amp; "]","") &amp; IF(E75&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E75 &amp; CHAR(10) &amp; "]","") &amp; IF(F75&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F75 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13133,10 +13133,10 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="G76" s="23" t="str">
         <f>"[Scene=" &amp; A76 &amp; IF(OR(B76&lt;&gt;"",C76&lt;&gt;"",D76&lt;&gt;""),CHAR(10),"") &amp; IF(B76&lt;&gt;"","[BeepBack=" &amp; B76 &amp; "]","") &amp; IF(C76&lt;&gt;"","[Connection=" &amp; C76 &amp; "]","") &amp; IF(D76&lt;&gt;"","[Timer=" &amp; D76 &amp; "]","") &amp; IF(E76&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E76 &amp; CHAR(10) &amp; "]","") &amp; IF(F76&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F76 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13160,10 +13160,10 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G77" s="23" t="str">
         <f t="shared" ref="G77:G83" si="3">"[Scene=" &amp; A77 &amp; IF(OR(B77&lt;&gt;"",C77&lt;&gt;"",D77&lt;&gt;""),CHAR(10),"") &amp; IF(B77&lt;&gt;"","[BeepBack=" &amp; B77 &amp; "]","") &amp; IF(C77&lt;&gt;"","[Connection=" &amp; C77 &amp; "]","") &amp; IF(D77&lt;&gt;"","[Timer=" &amp; D77 &amp; "]","") &amp; IF(E77&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E77 &amp; CHAR(10) &amp; "]","") &amp; IF(F77&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F77 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13188,10 +13188,10 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G78" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13217,10 +13217,10 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G79" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13246,10 +13246,10 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G80" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13274,10 +13274,10 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G81" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13305,10 +13305,10 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G82" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13338,10 +13338,10 @@
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G83" s="24" t="str">
         <f t="shared" si="3"/>
@@ -13371,10 +13371,10 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G84" s="23" t="str">
         <f t="shared" ref="G84:G92" si="4">"[Scene=" &amp; A84 &amp; IF(OR(B84&lt;&gt;"",C84&lt;&gt;"",D84&lt;&gt;""),CHAR(10),"") &amp; IF(B84&lt;&gt;"","[BeepBack=" &amp; B84 &amp; "]","") &amp; IF(C84&lt;&gt;"","[Connection=" &amp; C84 &amp; "]","") &amp; IF(D84&lt;&gt;"","[Timer=" &amp; D84 &amp; "]","") &amp; IF(E84&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E84 &amp; CHAR(10) &amp; "]","") &amp; IF(F84&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F84 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13403,10 +13403,10 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="G85" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13430,10 +13430,10 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="G86" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13459,10 +13459,10 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G87" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13487,10 +13487,10 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13516,10 +13516,10 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G89" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13544,10 +13544,10 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G90" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13572,10 +13572,10 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="G91" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13602,10 +13602,10 @@
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G92" s="24" t="str">
         <f t="shared" si="4"/>
@@ -13635,10 +13635,10 @@
         <v>10</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="G93" s="23" t="str">
         <f t="shared" ref="G93:G135" si="5">"[Scene=" &amp; A93 &amp; IF(OR(B93&lt;&gt;"",C93&lt;&gt;"",D93&lt;&gt;""),CHAR(10),"") &amp; IF(B93&lt;&gt;"","[BeepBack=" &amp; B93 &amp; "]","") &amp; IF(C93&lt;&gt;"","[Connection=" &amp; C93 &amp; "]","") &amp; IF(D93&lt;&gt;"","[Timer=" &amp; D93 &amp; "]","") &amp; IF(E93&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E93 &amp; CHAR(10) &amp; "]","") &amp; IF(F93&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F93 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13669,10 +13669,10 @@
         <v>10</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G94" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13702,10 +13702,10 @@
         <v>10</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G95" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13737,10 +13737,10 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G96" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13768,10 +13768,10 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="G97" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13799,10 +13799,10 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G98" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13829,10 +13829,10 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G99" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13860,10 +13860,10 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13894,10 +13894,10 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G101" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13926,10 +13926,10 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G102" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13957,10 +13957,10 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G103" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13989,10 +13989,10 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G104" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14017,10 +14017,10 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="G105" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14047,10 +14047,10 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14074,10 +14074,10 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G107" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14102,10 +14102,10 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G108" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14130,10 +14130,10 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G109" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14158,10 +14158,10 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G110" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14188,10 +14188,10 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G111" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14216,10 +14216,10 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G112" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14243,10 +14243,10 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G113" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14271,10 +14271,10 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G114" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14300,10 +14300,10 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G115" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14328,10 +14328,10 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G116" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14356,10 +14356,10 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G117" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14382,10 +14382,10 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="G118" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14408,10 +14408,10 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G119" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14438,10 +14438,10 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G120" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14466,10 +14466,10 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="G121" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14495,10 +14495,10 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G122" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14523,10 +14523,10 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G123" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14551,10 +14551,10 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G124" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14580,10 +14580,10 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G125" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14609,10 +14609,10 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G126" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14636,10 +14636,10 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="G127" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14663,10 +14663,10 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G128" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14693,10 +14693,10 @@
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G129" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14724,10 +14724,10 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G130" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14756,10 +14756,10 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G131" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14782,10 +14782,10 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F132" s="8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G132" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14809,10 +14809,10 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F133" s="8" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G133" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14839,10 +14839,10 @@
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G134" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14871,10 +14871,10 @@
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G135" s="23" t="str">
         <f t="shared" si="5"/>

</xml_diff>